<commit_message>
Dates added to excel
</commit_message>
<xml_diff>
--- a/tabela.xlsx
+++ b/tabela.xlsx
@@ -397,3304 +397,3739 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G145"/>
+  <dimension ref="A1:H145"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B1" t="str">
         <v/>
       </c>
-      <c r="B1" t="str">
+      <c r="C1" t="str">
         <v>FIXING I</v>
       </c>
-      <c r="C1" t="str">
+      <c r="D1" t="str">
         <v>FIXING II</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E1" t="str">
         <v>Notowania ciągłe</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B2" t="str">
         <v>Czas</v>
       </c>
-      <c r="B2" t="str">
+      <c r="C2" t="str">
         <v>Kurs (PLN/MWh)</v>
       </c>
-      <c r="C2" t="str">
+      <c r="D2" t="str">
         <v>Wolumen (MWh)</v>
       </c>
-      <c r="D2" t="str">
+      <c r="E2" t="str">
         <v>Kurs (PLN/MWh)</v>
       </c>
-      <c r="E2" t="str">
+      <c r="F2" t="str">
         <v>Wolumen (MWh)</v>
       </c>
-      <c r="F2" t="str">
+      <c r="G2" t="str">
         <v>Kurs (PLN/MWh)</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" t="str">
         <v>Wolumen (MWh)</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B3" t="str">
         <v>0-1</v>
       </c>
-      <c r="B3" t="str">
+      <c r="C3" t="str">
         <v>433,00</v>
       </c>
-      <c r="C3" t="str">
+      <c r="D3" t="str">
         <v>2883,3</v>
       </c>
-      <c r="D3" t="str">
+      <c r="E3" t="str">
         <v>433,56</v>
       </c>
-      <c r="E3" t="str">
+      <c r="F3" t="str">
         <v>1128</v>
       </c>
-      <c r="F3" t="str">
+      <c r="G3" t="str">
         <v>423,00</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" t="str">
         <v>20</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B4" t="str">
         <v>1-2</v>
       </c>
-      <c r="B4" t="str">
+      <c r="C4" t="str">
         <v>380,00</v>
       </c>
-      <c r="C4" t="str">
+      <c r="D4" t="str">
         <v>2776,3</v>
       </c>
-      <c r="D4" t="str">
+      <c r="E4" t="str">
         <v>375,23</v>
       </c>
-      <c r="E4" t="str">
+      <c r="F4" t="str">
         <v>648,9</v>
       </c>
-      <c r="F4" t="str">
-        <v>-</v>
-      </c>
       <c r="G4" t="str">
+        <v>-</v>
+      </c>
+      <c r="H4" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B5" t="str">
         <v>2-3</v>
       </c>
-      <c r="B5" t="str">
+      <c r="C5" t="str">
         <v>389,50</v>
       </c>
-      <c r="C5" t="str">
+      <c r="D5" t="str">
         <v>2590,4</v>
       </c>
-      <c r="D5" t="str">
+      <c r="E5" t="str">
         <v>380,90</v>
       </c>
-      <c r="E5" t="str">
+      <c r="F5" t="str">
         <v>835,2</v>
       </c>
-      <c r="F5" t="str">
-        <v>-</v>
-      </c>
       <c r="G5" t="str">
+        <v>-</v>
+      </c>
+      <c r="H5" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B6" t="str">
         <v>3-4</v>
       </c>
-      <c r="B6" t="str">
+      <c r="C6" t="str">
         <v>376,00</v>
       </c>
-      <c r="C6" t="str">
+      <c r="D6" t="str">
         <v>2722,2</v>
       </c>
-      <c r="D6" t="str">
+      <c r="E6" t="str">
         <v>375,37</v>
       </c>
-      <c r="E6" t="str">
+      <c r="F6" t="str">
         <v>1042,4</v>
       </c>
-      <c r="F6" t="str">
-        <v>-</v>
-      </c>
       <c r="G6" t="str">
+        <v>-</v>
+      </c>
+      <c r="H6" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B7" t="str">
         <v>4-5</v>
       </c>
-      <c r="B7" t="str">
+      <c r="C7" t="str">
         <v>381,08</v>
       </c>
-      <c r="C7" t="str">
+      <c r="D7" t="str">
         <v>2797,7</v>
       </c>
-      <c r="D7" t="str">
+      <c r="E7" t="str">
         <v>375,20</v>
       </c>
-      <c r="E7" t="str">
+      <c r="F7" t="str">
         <v>752,8</v>
       </c>
-      <c r="F7" t="str">
-        <v>-</v>
-      </c>
       <c r="G7" t="str">
+        <v>-</v>
+      </c>
+      <c r="H7" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B8" t="str">
         <v>5-6</v>
       </c>
-      <c r="B8" t="str">
+      <c r="C8" t="str">
         <v>393,55</v>
       </c>
-      <c r="C8" t="str">
+      <c r="D8" t="str">
         <v>3007,5</v>
       </c>
-      <c r="D8" t="str">
+      <c r="E8" t="str">
         <v>431,02</v>
       </c>
-      <c r="E8" t="str">
+      <c r="F8" t="str">
         <v>737,5</v>
       </c>
-      <c r="F8" t="str">
-        <v>-</v>
-      </c>
       <c r="G8" t="str">
+        <v>-</v>
+      </c>
+      <c r="H8" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B9" t="str">
         <v>6-7</v>
       </c>
-      <c r="B9" t="str">
+      <c r="C9" t="str">
         <v>509,11</v>
       </c>
-      <c r="C9" t="str">
+      <c r="D9" t="str">
         <v>3317,4</v>
       </c>
-      <c r="D9" t="str">
+      <c r="E9" t="str">
         <v>490,78</v>
       </c>
-      <c r="E9" t="str">
+      <c r="F9" t="str">
         <v>1461,1</v>
       </c>
-      <c r="F9" t="str">
-        <v>-</v>
-      </c>
       <c r="G9" t="str">
+        <v>-</v>
+      </c>
+      <c r="H9" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B10" t="str">
         <v>7-8</v>
       </c>
-      <c r="B10" t="str">
+      <c r="C10" t="str">
         <v>506,40</v>
       </c>
-      <c r="C10" t="str">
+      <c r="D10" t="str">
         <v>2930</v>
       </c>
-      <c r="D10" t="str">
+      <c r="E10" t="str">
         <v>486,05</v>
       </c>
-      <c r="E10" t="str">
+      <c r="F10" t="str">
         <v>1117,8</v>
       </c>
-      <c r="F10" t="str">
-        <v>-</v>
-      </c>
       <c r="G10" t="str">
+        <v>-</v>
+      </c>
+      <c r="H10" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B11" t="str">
         <v>8-9</v>
       </c>
-      <c r="B11" t="str">
+      <c r="C11" t="str">
         <v>416,30</v>
       </c>
-      <c r="C11" t="str">
+      <c r="D11" t="str">
         <v>3061,2</v>
       </c>
-      <c r="D11" t="str">
+      <c r="E11" t="str">
         <v>423,86</v>
       </c>
-      <c r="E11" t="str">
+      <c r="F11" t="str">
         <v>743,1</v>
       </c>
-      <c r="F11" t="str">
-        <v>-</v>
-      </c>
       <c r="G11" t="str">
+        <v>-</v>
+      </c>
+      <c r="H11" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B12" t="str">
         <v>9-10</v>
       </c>
-      <c r="B12" t="str">
+      <c r="C12" t="str">
         <v>283,99</v>
       </c>
-      <c r="C12" t="str">
+      <c r="D12" t="str">
         <v>3908,2</v>
       </c>
-      <c r="D12" t="str">
+      <c r="E12" t="str">
         <v>283,87</v>
       </c>
-      <c r="E12" t="str">
+      <c r="F12" t="str">
         <v>1557,5</v>
       </c>
-      <c r="F12" t="str">
-        <v>-</v>
-      </c>
       <c r="G12" t="str">
+        <v>-</v>
+      </c>
+      <c r="H12" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B13" t="str">
         <v>10-11</v>
       </c>
-      <c r="B13" t="str">
+      <c r="C13" t="str">
         <v>180,11</v>
       </c>
-      <c r="C13" t="str">
+      <c r="D13" t="str">
         <v>5009</v>
       </c>
-      <c r="D13" t="str">
+      <c r="E13" t="str">
         <v>161,01</v>
       </c>
-      <c r="E13" t="str">
+      <c r="F13" t="str">
         <v>2102,5</v>
       </c>
-      <c r="F13" t="str">
-        <v>-</v>
-      </c>
       <c r="G13" t="str">
+        <v>-</v>
+      </c>
+      <c r="H13" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B14" t="str">
         <v>11-12</v>
       </c>
-      <c r="B14" t="str">
+      <c r="C14" t="str">
         <v>90,11</v>
       </c>
-      <c r="C14" t="str">
+      <c r="D14" t="str">
         <v>5265,3</v>
       </c>
-      <c r="D14" t="str">
+      <c r="E14" t="str">
         <v>33,64</v>
       </c>
-      <c r="E14" t="str">
+      <c r="F14" t="str">
         <v>2002,2</v>
       </c>
-      <c r="F14" t="str">
-        <v>-</v>
-      </c>
       <c r="G14" t="str">
+        <v>-</v>
+      </c>
+      <c r="H14" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B15" t="str">
         <v>12-13</v>
       </c>
-      <c r="B15" t="str">
+      <c r="C15" t="str">
         <v>30,00</v>
       </c>
-      <c r="C15" t="str">
+      <c r="D15" t="str">
         <v>5106,9</v>
       </c>
-      <c r="D15" t="str">
+      <c r="E15" t="str">
         <v>4,68</v>
       </c>
-      <c r="E15" t="str">
+      <c r="F15" t="str">
         <v>2081</v>
       </c>
-      <c r="F15" t="str">
+      <c r="G15" t="str">
         <v>30,00</v>
       </c>
-      <c r="G15" t="str">
+      <c r="H15" t="str">
         <v>1,6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B16" t="str">
         <v>13-14</v>
       </c>
-      <c r="B16" t="str">
+      <c r="C16" t="str">
         <v>10,11</v>
       </c>
-      <c r="C16" t="str">
+      <c r="D16" t="str">
         <v>4834,2</v>
       </c>
-      <c r="D16" t="str">
+      <c r="E16" t="str">
         <v>0,04</v>
       </c>
-      <c r="E16" t="str">
+      <c r="F16" t="str">
         <v>1963,5</v>
       </c>
-      <c r="F16" t="str">
+      <c r="G16" t="str">
         <v>10,11</v>
       </c>
-      <c r="G16" t="str">
+      <c r="H16" t="str">
         <v>3,6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B17" t="str">
         <v>14-15</v>
       </c>
-      <c r="B17" t="str">
+      <c r="C17" t="str">
         <v>21,40</v>
       </c>
-      <c r="C17" t="str">
+      <c r="D17" t="str">
         <v>4585,7</v>
       </c>
-      <c r="D17" t="str">
+      <c r="E17" t="str">
         <v>7,46</v>
       </c>
-      <c r="E17" t="str">
+      <c r="F17" t="str">
         <v>1710,2</v>
       </c>
-      <c r="F17" t="str">
+      <c r="G17" t="str">
         <v>21,40</v>
       </c>
-      <c r="G17" t="str">
+      <c r="H17" t="str">
         <v>4,8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B18" t="str">
         <v>15-16</v>
       </c>
-      <c r="B18" t="str">
+      <c r="C18" t="str">
         <v>165,00</v>
       </c>
-      <c r="C18" t="str">
+      <c r="D18" t="str">
         <v>3905,8</v>
       </c>
-      <c r="D18" t="str">
+      <c r="E18" t="str">
         <v>60,19</v>
       </c>
-      <c r="E18" t="str">
+      <c r="F18" t="str">
         <v>919,4</v>
       </c>
-      <c r="F18" t="str">
+      <c r="G18" t="str">
         <v>165,00</v>
       </c>
-      <c r="G18" t="str">
+      <c r="H18" t="str">
         <v>20</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B19" t="str">
         <v>16-17</v>
       </c>
-      <c r="B19" t="str">
+      <c r="C19" t="str">
         <v>315,99</v>
       </c>
-      <c r="C19" t="str">
+      <c r="D19" t="str">
         <v>3216,1</v>
       </c>
-      <c r="D19" t="str">
+      <c r="E19" t="str">
         <v>333,67</v>
       </c>
-      <c r="E19" t="str">
+      <c r="F19" t="str">
         <v>729</v>
       </c>
-      <c r="F19" t="str">
+      <c r="G19" t="str">
         <v>316,00</v>
       </c>
-      <c r="G19" t="str">
+      <c r="H19" t="str">
         <v>11</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B20" t="str">
         <v>17-18</v>
       </c>
-      <c r="B20" t="str">
+      <c r="C20" t="str">
         <v>380,60</v>
       </c>
-      <c r="C20" t="str">
+      <c r="D20" t="str">
         <v>3471,4</v>
       </c>
-      <c r="D20" t="str">
+      <c r="E20" t="str">
         <v>352,40</v>
       </c>
-      <c r="E20" t="str">
+      <c r="F20" t="str">
         <v>1193,6</v>
       </c>
-      <c r="F20" t="str">
-        <v>-</v>
-      </c>
       <c r="G20" t="str">
+        <v>-</v>
+      </c>
+      <c r="H20" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B21" t="str">
         <v>18-19</v>
       </c>
-      <c r="B21" t="str">
+      <c r="C21" t="str">
         <v>481,00</v>
       </c>
-      <c r="C21" t="str">
+      <c r="D21" t="str">
         <v>3695,3</v>
       </c>
-      <c r="D21" t="str">
+      <c r="E21" t="str">
         <v>435,64</v>
       </c>
-      <c r="E21" t="str">
+      <c r="F21" t="str">
         <v>2383,8</v>
       </c>
-      <c r="F21" t="str">
-        <v>-</v>
-      </c>
       <c r="G21" t="str">
+        <v>-</v>
+      </c>
+      <c r="H21" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B22" t="str">
         <v>19-20</v>
       </c>
-      <c r="B22" t="str">
+      <c r="C22" t="str">
         <v>682,00</v>
       </c>
-      <c r="C22" t="str">
+      <c r="D22" t="str">
         <v>4475</v>
       </c>
-      <c r="D22" t="str">
+      <c r="E22" t="str">
         <v>656,89</v>
       </c>
-      <c r="E22" t="str">
+      <c r="F22" t="str">
         <v>2695,9</v>
       </c>
-      <c r="F22" t="str">
+      <c r="G22" t="str">
         <v>672,75</v>
       </c>
-      <c r="G22" t="str">
+      <c r="H22" t="str">
         <v>91</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B23" t="str">
         <v>20-21</v>
       </c>
-      <c r="B23" t="str">
+      <c r="C23" t="str">
         <v>853,40</v>
       </c>
-      <c r="C23" t="str">
+      <c r="D23" t="str">
         <v>4636,4</v>
       </c>
-      <c r="D23" t="str">
+      <c r="E23" t="str">
         <v>901,75</v>
       </c>
-      <c r="E23" t="str">
+      <c r="F23" t="str">
         <v>2699,1</v>
       </c>
-      <c r="F23" t="str">
+      <c r="G23" t="str">
         <v>851,31</v>
       </c>
-      <c r="G23" t="str">
+      <c r="H23" t="str">
         <v>180,2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B24" t="str">
         <v>21-22</v>
       </c>
-      <c r="B24" t="str">
+      <c r="C24" t="str">
         <v>720,00</v>
       </c>
-      <c r="C24" t="str">
+      <c r="D24" t="str">
         <v>4560,7</v>
       </c>
-      <c r="D24" t="str">
+      <c r="E24" t="str">
         <v>650,61</v>
       </c>
-      <c r="E24" t="str">
+      <c r="F24" t="str">
         <v>2968,2</v>
       </c>
-      <c r="F24" t="str">
+      <c r="G24" t="str">
         <v>711,18</v>
       </c>
-      <c r="G24" t="str">
+      <c r="H24" t="str">
         <v>80,5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B25" t="str">
         <v>22-23</v>
       </c>
-      <c r="B25" t="str">
+      <c r="C25" t="str">
         <v>549,00</v>
       </c>
-      <c r="C25" t="str">
+      <c r="D25" t="str">
         <v>4383,7</v>
       </c>
-      <c r="D25" t="str">
+      <c r="E25" t="str">
         <v>509,95</v>
       </c>
-      <c r="E25" t="str">
+      <c r="F25" t="str">
         <v>3388,4</v>
       </c>
-      <c r="F25" t="str">
+      <c r="G25" t="str">
         <v>540,00</v>
       </c>
-      <c r="G25" t="str">
+      <c r="H25" t="str">
         <v>30</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B26" t="str">
         <v>23-24</v>
       </c>
-      <c r="B26" t="str">
+      <c r="C26" t="str">
         <v>458,00</v>
       </c>
-      <c r="C26" t="str">
+      <c r="D26" t="str">
         <v>3816,3</v>
       </c>
-      <c r="D26" t="str">
+      <c r="E26" t="str">
         <v>424,99</v>
       </c>
-      <c r="E26" t="str">
+      <c r="F26" t="str">
         <v>2886</v>
       </c>
-      <c r="F26" t="str">
+      <c r="G26" t="str">
         <v>455,00</v>
       </c>
-      <c r="G26" t="str">
+      <c r="H26" t="str">
         <v>30</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B27" t="str">
         <v>Min.</v>
       </c>
-      <c r="B27" t="str">
+      <c r="C27" t="str">
         <v>10,11</v>
       </c>
-      <c r="C27" t="str">
-        <v>-</v>
-      </c>
       <c r="D27" t="str">
+        <v>-</v>
+      </c>
+      <c r="E27" t="str">
         <v>0,04</v>
       </c>
-      <c r="E27" t="str">
-        <v>-</v>
-      </c>
       <c r="F27" t="str">
+        <v>-</v>
+      </c>
+      <c r="G27" t="str">
         <v>10,11</v>
       </c>
-      <c r="G27" t="str">
+      <c r="H27" t="str">
         <v>-</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B28" t="str">
         <v>Maks.</v>
       </c>
-      <c r="B28" t="str">
+      <c r="C28" t="str">
         <v>853,40</v>
       </c>
-      <c r="C28" t="str">
-        <v>-</v>
-      </c>
       <c r="D28" t="str">
+        <v>-</v>
+      </c>
+      <c r="E28" t="str">
         <v>901,75</v>
       </c>
-      <c r="E28" t="str">
-        <v>-</v>
-      </c>
       <c r="F28" t="str">
+        <v>-</v>
+      </c>
+      <c r="G28" t="str">
         <v>851,31</v>
       </c>
-      <c r="G28" t="str">
+      <c r="H28" t="str">
         <v>-</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
+        <v>29-07-2024</v>
+      </c>
+      <c r="B29" t="str">
         <v>Suma</v>
       </c>
-      <c r="B29" t="str">
+      <c r="C29" t="str">
         <v/>
       </c>
-      <c r="C29" t="str">
+      <c r="D29" t="str">
         <v>90 956</v>
       </c>
-      <c r="D29" t="str">
+      <c r="E29" t="str">
         <v/>
       </c>
-      <c r="E29" t="str">
+      <c r="F29" t="str">
         <v>39 747,1</v>
       </c>
-      <c r="F29" t="str">
+      <c r="G29" t="str">
         <v/>
       </c>
-      <c r="G29" t="str">
+      <c r="H29" t="str">
         <v>472,7</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B30" t="str">
         <v/>
       </c>
-      <c r="B30" t="str">
+      <c r="C30" t="str">
         <v>FIXING I</v>
       </c>
-      <c r="C30" t="str">
+      <c r="D30" t="str">
         <v>FIXING II</v>
       </c>
-      <c r="D30" t="str">
+      <c r="E30" t="str">
         <v>Notowania ciągłe</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B31" t="str">
         <v>Czas</v>
       </c>
-      <c r="B31" t="str">
+      <c r="C31" t="str">
         <v>Kurs (PLN/MWh)</v>
       </c>
-      <c r="C31" t="str">
+      <c r="D31" t="str">
         <v>Wolumen (MWh)</v>
       </c>
-      <c r="D31" t="str">
+      <c r="E31" t="str">
         <v>Kurs (PLN/MWh)</v>
       </c>
-      <c r="E31" t="str">
+      <c r="F31" t="str">
         <v>Wolumen (MWh)</v>
       </c>
-      <c r="F31" t="str">
+      <c r="G31" t="str">
         <v>Kurs (PLN/MWh)</v>
       </c>
-      <c r="G31" t="str">
+      <c r="H31" t="str">
         <v>Wolumen (MWh)</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B32" t="str">
         <v>0-1</v>
       </c>
-      <c r="B32" t="str">
+      <c r="C32" t="str">
         <v>473,14</v>
       </c>
-      <c r="C32" t="str">
+      <c r="D32" t="str">
         <v>3590,6</v>
       </c>
-      <c r="D32" t="str">
+      <c r="E32" t="str">
         <v>423,66</v>
       </c>
-      <c r="E32" t="str">
+      <c r="F32" t="str">
         <v>3017,3</v>
       </c>
-      <c r="F32" t="str">
+      <c r="G32" t="str">
         <v>463,00</v>
       </c>
-      <c r="G32" t="str">
+      <c r="H32" t="str">
         <v>40</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B33" t="str">
         <v>1-2</v>
       </c>
-      <c r="B33" t="str">
+      <c r="C33" t="str">
         <v>418,00</v>
       </c>
-      <c r="C33" t="str">
+      <c r="D33" t="str">
         <v>3467,1</v>
       </c>
-      <c r="D33" t="str">
+      <c r="E33" t="str">
         <v>372,85</v>
       </c>
-      <c r="E33" t="str">
+      <c r="F33" t="str">
         <v>2630</v>
       </c>
-      <c r="F33" t="str">
-        <v>-</v>
-      </c>
       <c r="G33" t="str">
+        <v>-</v>
+      </c>
+      <c r="H33" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B34" t="str">
         <v>2-3</v>
       </c>
-      <c r="B34" t="str">
+      <c r="C34" t="str">
         <v>406,26</v>
       </c>
-      <c r="C34" t="str">
+      <c r="D34" t="str">
         <v>3180,1</v>
       </c>
-      <c r="D34" t="str">
+      <c r="E34" t="str">
         <v>363,45</v>
       </c>
-      <c r="E34" t="str">
+      <c r="F34" t="str">
         <v>2418,6</v>
       </c>
-      <c r="F34" t="str">
-        <v>-</v>
-      </c>
       <c r="G34" t="str">
+        <v>-</v>
+      </c>
+      <c r="H34" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B35" t="str">
         <v>3-4</v>
       </c>
-      <c r="B35" t="str">
+      <c r="C35" t="str">
         <v>407,00</v>
       </c>
-      <c r="C35" t="str">
+      <c r="D35" t="str">
         <v>3286,2</v>
       </c>
-      <c r="D35" t="str">
+      <c r="E35" t="str">
         <v>357,63</v>
       </c>
-      <c r="E35" t="str">
+      <c r="F35" t="str">
         <v>2539,7</v>
       </c>
-      <c r="F35" t="str">
-        <v>-</v>
-      </c>
       <c r="G35" t="str">
+        <v>-</v>
+      </c>
+      <c r="H35" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B36" t="str">
         <v>4-5</v>
       </c>
-      <c r="B36" t="str">
+      <c r="C36" t="str">
         <v>408,00</v>
       </c>
-      <c r="C36" t="str">
+      <c r="D36" t="str">
         <v>3260,6</v>
       </c>
-      <c r="D36" t="str">
+      <c r="E36" t="str">
         <v>389,06</v>
       </c>
-      <c r="E36" t="str">
+      <c r="F36" t="str">
         <v>2243,2</v>
       </c>
-      <c r="F36" t="str">
-        <v>-</v>
-      </c>
       <c r="G36" t="str">
+        <v>-</v>
+      </c>
+      <c r="H36" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B37" t="str">
         <v>5-6</v>
       </c>
-      <c r="B37" t="str">
+      <c r="C37" t="str">
         <v>443,55</v>
       </c>
-      <c r="C37" t="str">
+      <c r="D37" t="str">
         <v>3268,3</v>
       </c>
-      <c r="D37" t="str">
+      <c r="E37" t="str">
         <v>435,91</v>
       </c>
-      <c r="E37" t="str">
+      <c r="F37" t="str">
         <v>1779,2</v>
       </c>
-      <c r="F37" t="str">
+      <c r="G37" t="str">
         <v>443,55</v>
       </c>
-      <c r="G37" t="str">
+      <c r="H37" t="str">
         <v>25</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B38" t="str">
         <v>6-7</v>
       </c>
-      <c r="B38" t="str">
+      <c r="C38" t="str">
         <v>550,00</v>
       </c>
-      <c r="C38" t="str">
+      <c r="D38" t="str">
         <v>3763,2</v>
       </c>
-      <c r="D38" t="str">
+      <c r="E38" t="str">
         <v>494,05</v>
       </c>
-      <c r="E38" t="str">
+      <c r="F38" t="str">
         <v>2334,5</v>
       </c>
-      <c r="F38" t="str">
+      <c r="G38" t="str">
         <v>544,95</v>
       </c>
-      <c r="G38" t="str">
+      <c r="H38" t="str">
         <v>10</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B39" t="str">
         <v>7-8</v>
       </c>
-      <c r="B39" t="str">
+      <c r="C39" t="str">
         <v>530,00</v>
       </c>
-      <c r="C39" t="str">
+      <c r="D39" t="str">
         <v>2890,9</v>
       </c>
-      <c r="D39" t="str">
+      <c r="E39" t="str">
         <v>469,38</v>
       </c>
-      <c r="E39" t="str">
+      <c r="F39" t="str">
         <v>1447</v>
       </c>
-      <c r="F39" t="str">
-        <v>-</v>
-      </c>
       <c r="G39" t="str">
+        <v>-</v>
+      </c>
+      <c r="H39" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B40" t="str">
         <v>8-9</v>
       </c>
-      <c r="B40" t="str">
+      <c r="C40" t="str">
         <v>420,00</v>
       </c>
-      <c r="C40" t="str">
+      <c r="D40" t="str">
         <v>3040,8</v>
       </c>
-      <c r="D40" t="str">
+      <c r="E40" t="str">
         <v>408,39</v>
       </c>
-      <c r="E40" t="str">
+      <c r="F40" t="str">
         <v>1000,8</v>
       </c>
-      <c r="F40" t="str">
-        <v>-</v>
-      </c>
       <c r="G40" t="str">
+        <v>-</v>
+      </c>
+      <c r="H40" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B41" t="str">
         <v>9-10</v>
       </c>
-      <c r="B41" t="str">
+      <c r="C41" t="str">
         <v>303,99</v>
       </c>
-      <c r="C41" t="str">
+      <c r="D41" t="str">
         <v>3372,1</v>
       </c>
-      <c r="D41" t="str">
+      <c r="E41" t="str">
         <v>339,12</v>
       </c>
-      <c r="E41" t="str">
+      <c r="F41" t="str">
         <v>1091,7</v>
       </c>
-      <c r="F41" t="str">
+      <c r="G41" t="str">
         <v>294,00</v>
       </c>
-      <c r="G41" t="str">
+      <c r="H41" t="str">
         <v>10</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B42" t="str">
         <v>10-11</v>
       </c>
-      <c r="B42" t="str">
+      <c r="C42" t="str">
         <v>198,12</v>
       </c>
-      <c r="C42" t="str">
+      <c r="D42" t="str">
         <v>4010,7</v>
       </c>
-      <c r="D42" t="str">
+      <c r="E42" t="str">
         <v>239,76</v>
       </c>
-      <c r="E42" t="str">
+      <c r="F42" t="str">
         <v>1662,9</v>
       </c>
-      <c r="F42" t="str">
-        <v>-</v>
-      </c>
       <c r="G42" t="str">
+        <v>-</v>
+      </c>
+      <c r="H42" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B43" t="str">
         <v>11-12</v>
       </c>
-      <c r="B43" t="str">
+      <c r="C43" t="str">
         <v>105,95</v>
       </c>
-      <c r="C43" t="str">
+      <c r="D43" t="str">
         <v>4484,2</v>
       </c>
-      <c r="D43" t="str">
+      <c r="E43" t="str">
         <v>143,53</v>
       </c>
-      <c r="E43" t="str">
+      <c r="F43" t="str">
         <v>1981,6</v>
       </c>
-      <c r="F43" t="str">
-        <v>-</v>
-      </c>
       <c r="G43" t="str">
+        <v>-</v>
+      </c>
+      <c r="H43" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B44" t="str">
         <v>12-13</v>
       </c>
-      <c r="B44" t="str">
+      <c r="C44" t="str">
         <v>70,00</v>
       </c>
-      <c r="C44" t="str">
+      <c r="D44" t="str">
         <v>4324,5</v>
       </c>
-      <c r="D44" t="str">
+      <c r="E44" t="str">
         <v>107,68</v>
       </c>
-      <c r="E44" t="str">
+      <c r="F44" t="str">
         <v>1695,8</v>
       </c>
-      <c r="F44" t="str">
-        <v>-</v>
-      </c>
       <c r="G44" t="str">
+        <v>-</v>
+      </c>
+      <c r="H44" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B45" t="str">
         <v>13-14</v>
       </c>
-      <c r="B45" t="str">
+      <c r="C45" t="str">
         <v>70,00</v>
       </c>
-      <c r="C45" t="str">
+      <c r="D45" t="str">
         <v>4096,6</v>
       </c>
-      <c r="D45" t="str">
+      <c r="E45" t="str">
         <v>71,81</v>
       </c>
-      <c r="E45" t="str">
+      <c r="F45" t="str">
         <v>1335,4</v>
       </c>
-      <c r="F45" t="str">
-        <v>-</v>
-      </c>
       <c r="G45" t="str">
+        <v>-</v>
+      </c>
+      <c r="H45" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B46" t="str">
         <v>14-15</v>
       </c>
-      <c r="B46" t="str">
+      <c r="C46" t="str">
         <v>100,00</v>
       </c>
-      <c r="C46" t="str">
+      <c r="D46" t="str">
         <v>3791</v>
       </c>
-      <c r="D46" t="str">
+      <c r="E46" t="str">
         <v>98,70</v>
       </c>
-      <c r="E46" t="str">
+      <c r="F46" t="str">
         <v>1106,5</v>
       </c>
-      <c r="F46" t="str">
-        <v>-</v>
-      </c>
       <c r="G46" t="str">
+        <v>-</v>
+      </c>
+      <c r="H46" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B47" t="str">
         <v>15-16</v>
       </c>
-      <c r="B47" t="str">
+      <c r="C47" t="str">
         <v>239,99</v>
       </c>
-      <c r="C47" t="str">
+      <c r="D47" t="str">
         <v>3223,9</v>
       </c>
-      <c r="D47" t="str">
+      <c r="E47" t="str">
         <v>175,36</v>
       </c>
-      <c r="E47" t="str">
+      <c r="F47" t="str">
         <v>961,4</v>
       </c>
-      <c r="F47" t="str">
-        <v>-</v>
-      </c>
       <c r="G47" t="str">
+        <v>-</v>
+      </c>
+      <c r="H47" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B48" t="str">
         <v>16-17</v>
       </c>
-      <c r="B48" t="str">
+      <c r="C48" t="str">
         <v>370,60</v>
       </c>
-      <c r="C48" t="str">
+      <c r="D48" t="str">
         <v>2768,7</v>
       </c>
-      <c r="D48" t="str">
+      <c r="E48" t="str">
         <v>307,32</v>
       </c>
-      <c r="E48" t="str">
+      <c r="F48" t="str">
         <v>705,9</v>
       </c>
-      <c r="F48" t="str">
+      <c r="G48" t="str">
         <v>370,60</v>
       </c>
-      <c r="G48" t="str">
+      <c r="H48" t="str">
         <v>17,8</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B49" t="str">
         <v>17-18</v>
       </c>
-      <c r="B49" t="str">
+      <c r="C49" t="str">
         <v>379,00</v>
       </c>
-      <c r="C49" t="str">
+      <c r="D49" t="str">
         <v>3235</v>
       </c>
-      <c r="D49" t="str">
+      <c r="E49" t="str">
         <v>343,68</v>
       </c>
-      <c r="E49" t="str">
+      <c r="F49" t="str">
         <v>1541,7</v>
       </c>
-      <c r="F49" t="str">
-        <v>-</v>
-      </c>
       <c r="G49" t="str">
+        <v>-</v>
+      </c>
+      <c r="H49" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B50" t="str">
         <v>18-19</v>
       </c>
-      <c r="B50" t="str">
+      <c r="C50" t="str">
         <v>499,40</v>
       </c>
-      <c r="C50" t="str">
+      <c r="D50" t="str">
         <v>3681,1</v>
       </c>
-      <c r="D50" t="str">
+      <c r="E50" t="str">
         <v>405,64</v>
       </c>
-      <c r="E50" t="str">
+      <c r="F50" t="str">
         <v>2278,4</v>
       </c>
-      <c r="F50" t="str">
+      <c r="G50" t="str">
         <v>487,00</v>
       </c>
-      <c r="G50" t="str">
+      <c r="H50" t="str">
         <v>10</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B51" t="str">
         <v>19-20</v>
       </c>
-      <c r="B51" t="str">
+      <c r="C51" t="str">
         <v>632,00</v>
       </c>
-      <c r="C51" t="str">
+      <c r="D51" t="str">
         <v>4227,4</v>
       </c>
-      <c r="D51" t="str">
+      <c r="E51" t="str">
         <v>513,65</v>
       </c>
-      <c r="E51" t="str">
+      <c r="F51" t="str">
         <v>2357,2</v>
       </c>
-      <c r="F51" t="str">
+      <c r="G51" t="str">
         <v>633,33</v>
       </c>
-      <c r="G51" t="str">
+      <c r="H51" t="str">
         <v>45</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B52" t="str">
         <v>20-21</v>
       </c>
-      <c r="B52" t="str">
+      <c r="C52" t="str">
         <v>825,00</v>
       </c>
-      <c r="C52" t="str">
+      <c r="D52" t="str">
         <v>4789,1</v>
       </c>
-      <c r="D52" t="str">
+      <c r="E52" t="str">
         <v>690,49</v>
       </c>
-      <c r="E52" t="str">
+      <c r="F52" t="str">
         <v>2294,2</v>
       </c>
-      <c r="F52" t="str">
+      <c r="G52" t="str">
         <v>815,00</v>
       </c>
-      <c r="G52" t="str">
+      <c r="H52" t="str">
         <v>20</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B53" t="str">
         <v>21-22</v>
       </c>
-      <c r="B53" t="str">
+      <c r="C53" t="str">
         <v>634,00</v>
       </c>
-      <c r="C53" t="str">
+      <c r="D53" t="str">
         <v>4367,9</v>
       </c>
-      <c r="D53" t="str">
+      <c r="E53" t="str">
         <v>550,36</v>
       </c>
-      <c r="E53" t="str">
+      <c r="F53" t="str">
         <v>2593,6</v>
       </c>
-      <c r="F53" t="str">
+      <c r="G53" t="str">
         <v>623,45</v>
       </c>
-      <c r="G53" t="str">
+      <c r="H53" t="str">
         <v>22</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B54" t="str">
         <v>22-23</v>
       </c>
-      <c r="B54" t="str">
+      <c r="C54" t="str">
         <v>520,00</v>
       </c>
-      <c r="C54" t="str">
+      <c r="D54" t="str">
         <v>4665,8</v>
       </c>
-      <c r="D54" t="str">
+      <c r="E54" t="str">
         <v>520,57</v>
       </c>
-      <c r="E54" t="str">
+      <c r="F54" t="str">
         <v>3148</v>
       </c>
-      <c r="F54" t="str">
+      <c r="G54" t="str">
         <v>510,00</v>
       </c>
-      <c r="G54" t="str">
+      <c r="H54" t="str">
         <v>20</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B55" t="str">
         <v>23-24</v>
       </c>
-      <c r="B55" t="str">
+      <c r="C55" t="str">
         <v>443,80</v>
       </c>
-      <c r="C55" t="str">
+      <c r="D55" t="str">
         <v>3914,9</v>
       </c>
-      <c r="D55" t="str">
+      <c r="E55" t="str">
         <v>421,22</v>
       </c>
-      <c r="E55" t="str">
+      <c r="F55" t="str">
         <v>2836,2</v>
       </c>
-      <c r="F55" t="str">
+      <c r="G55" t="str">
         <v>433,00</v>
       </c>
-      <c r="G55" t="str">
+      <c r="H55" t="str">
         <v>20</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B56" t="str">
         <v>Min.</v>
       </c>
-      <c r="B56" t="str">
+      <c r="C56" t="str">
         <v>70,00</v>
       </c>
-      <c r="C56" t="str">
-        <v>-</v>
-      </c>
       <c r="D56" t="str">
+        <v>-</v>
+      </c>
+      <c r="E56" t="str">
         <v>71,81</v>
       </c>
-      <c r="E56" t="str">
-        <v>-</v>
-      </c>
       <c r="F56" t="str">
+        <v>-</v>
+      </c>
+      <c r="G56" t="str">
         <v>294,00</v>
       </c>
-      <c r="G56" t="str">
+      <c r="H56" t="str">
         <v>-</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B57" t="str">
         <v>Maks.</v>
       </c>
-      <c r="B57" t="str">
+      <c r="C57" t="str">
         <v>825,00</v>
       </c>
-      <c r="C57" t="str">
-        <v>-</v>
-      </c>
       <c r="D57" t="str">
+        <v>-</v>
+      </c>
+      <c r="E57" t="str">
         <v>690,49</v>
       </c>
-      <c r="E57" t="str">
-        <v>-</v>
-      </c>
       <c r="F57" t="str">
+        <v>-</v>
+      </c>
+      <c r="G57" t="str">
         <v>815,00</v>
       </c>
-      <c r="G57" t="str">
+      <c r="H57" t="str">
         <v>-</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
+        <v>30-07-2024</v>
+      </c>
+      <c r="B58" t="str">
         <v>Suma</v>
       </c>
-      <c r="B58" t="str">
+      <c r="C58" t="str">
         <v/>
       </c>
-      <c r="C58" t="str">
+      <c r="D58" t="str">
         <v>88 700,7</v>
       </c>
-      <c r="D58" t="str">
+      <c r="E58" t="str">
         <v/>
       </c>
-      <c r="E58" t="str">
+      <c r="F58" t="str">
         <v>47 000,8</v>
       </c>
-      <c r="F58" t="str">
+      <c r="G58" t="str">
         <v/>
       </c>
-      <c r="G58" t="str">
+      <c r="H58" t="str">
         <v>239,8</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B59" t="str">
         <v/>
       </c>
-      <c r="B59" t="str">
+      <c r="C59" t="str">
         <v>FIXING I</v>
       </c>
-      <c r="C59" t="str">
+      <c r="D59" t="str">
         <v>FIXING II</v>
       </c>
-      <c r="D59" t="str">
+      <c r="E59" t="str">
         <v>Notowania ciągłe</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B60" t="str">
         <v>Czas</v>
       </c>
-      <c r="B60" t="str">
+      <c r="C60" t="str">
         <v>Kurs (PLN/MWh)</v>
       </c>
-      <c r="C60" t="str">
+      <c r="D60" t="str">
         <v>Wolumen (MWh)</v>
       </c>
-      <c r="D60" t="str">
+      <c r="E60" t="str">
         <v>Kurs (PLN/MWh)</v>
       </c>
-      <c r="E60" t="str">
+      <c r="F60" t="str">
         <v>Wolumen (MWh)</v>
       </c>
-      <c r="F60" t="str">
+      <c r="G60" t="str">
         <v>Kurs (PLN/MWh)</v>
       </c>
-      <c r="G60" t="str">
+      <c r="H60" t="str">
         <v>Wolumen (MWh)</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B61" t="str">
         <v>0-1</v>
       </c>
-      <c r="B61" t="str">
+      <c r="C61" t="str">
         <v>450,00</v>
       </c>
-      <c r="C61" t="str">
+      <c r="D61" t="str">
         <v>3361,3</v>
       </c>
-      <c r="D61" t="str">
+      <c r="E61" t="str">
         <v>432,45</v>
       </c>
-      <c r="E61" t="str">
+      <c r="F61" t="str">
         <v>2720</v>
       </c>
-      <c r="F61" t="str">
+      <c r="G61" t="str">
         <v>440,00</v>
       </c>
-      <c r="G61" t="str">
+      <c r="H61" t="str">
         <v>20</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B62" t="str">
         <v>1-2</v>
       </c>
-      <c r="B62" t="str">
+      <c r="C62" t="str">
         <v>400,00</v>
       </c>
-      <c r="C62" t="str">
+      <c r="D62" t="str">
         <v>3116,8</v>
       </c>
-      <c r="D62" t="str">
+      <c r="E62" t="str">
         <v>374,52</v>
       </c>
-      <c r="E62" t="str">
+      <c r="F62" t="str">
         <v>2417,4</v>
       </c>
-      <c r="F62" t="str">
-        <v>-</v>
-      </c>
       <c r="G62" t="str">
+        <v>-</v>
+      </c>
+      <c r="H62" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B63" t="str">
         <v>2-3</v>
       </c>
-      <c r="B63" t="str">
+      <c r="C63" t="str">
         <v>390,00</v>
       </c>
-      <c r="C63" t="str">
+      <c r="D63" t="str">
         <v>2958,7</v>
       </c>
-      <c r="D63" t="str">
+      <c r="E63" t="str">
         <v>363,35</v>
       </c>
-      <c r="E63" t="str">
+      <c r="F63" t="str">
         <v>2386,8</v>
       </c>
-      <c r="F63" t="str">
-        <v>-</v>
-      </c>
       <c r="G63" t="str">
+        <v>-</v>
+      </c>
+      <c r="H63" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B64" t="str">
         <v>3-4</v>
       </c>
-      <c r="B64" t="str">
+      <c r="C64" t="str">
         <v>390,00</v>
       </c>
-      <c r="C64" t="str">
+      <c r="D64" t="str">
         <v>3007,3</v>
       </c>
-      <c r="D64" t="str">
+      <c r="E64" t="str">
         <v>363,35</v>
       </c>
-      <c r="E64" t="str">
+      <c r="F64" t="str">
         <v>2439,9</v>
       </c>
-      <c r="F64" t="str">
-        <v>-</v>
-      </c>
       <c r="G64" t="str">
+        <v>-</v>
+      </c>
+      <c r="H64" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B65" t="str">
         <v>4-5</v>
       </c>
-      <c r="B65" t="str">
+      <c r="C65" t="str">
         <v>397,20</v>
       </c>
-      <c r="C65" t="str">
+      <c r="D65" t="str">
         <v>3066,5</v>
       </c>
-      <c r="D65" t="str">
+      <c r="E65" t="str">
         <v>359,51</v>
       </c>
-      <c r="E65" t="str">
+      <c r="F65" t="str">
         <v>2467,6</v>
       </c>
-      <c r="F65" t="str">
-        <v>-</v>
-      </c>
       <c r="G65" t="str">
+        <v>-</v>
+      </c>
+      <c r="H65" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B66" t="str">
         <v>5-6</v>
       </c>
-      <c r="B66" t="str">
+      <c r="C66" t="str">
         <v>437,00</v>
       </c>
-      <c r="C66" t="str">
+      <c r="D66" t="str">
         <v>3229,3</v>
       </c>
-      <c r="D66" t="str">
+      <c r="E66" t="str">
         <v>437,43</v>
       </c>
-      <c r="E66" t="str">
+      <c r="F66" t="str">
         <v>2022,4</v>
       </c>
-      <c r="F66" t="str">
+      <c r="G66" t="str">
         <v>437,00</v>
       </c>
-      <c r="G66" t="str">
+      <c r="H66" t="str">
         <v>37,1</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B67" t="str">
         <v>6-7</v>
       </c>
-      <c r="B67" t="str">
+      <c r="C67" t="str">
         <v>530,00</v>
       </c>
-      <c r="C67" t="str">
+      <c r="D67" t="str">
         <v>3597,5</v>
       </c>
-      <c r="D67" t="str">
+      <c r="E67" t="str">
         <v>545,18</v>
       </c>
-      <c r="E67" t="str">
+      <c r="F67" t="str">
         <v>2178,7</v>
       </c>
-      <c r="F67" t="str">
-        <v>-</v>
-      </c>
       <c r="G67" t="str">
+        <v>-</v>
+      </c>
+      <c r="H67" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B68" t="str">
         <v>7-8</v>
       </c>
-      <c r="B68" t="str">
+      <c r="C68" t="str">
         <v>520,00</v>
       </c>
-      <c r="C68" t="str">
+      <c r="D68" t="str">
         <v>3013,4</v>
       </c>
-      <c r="D68" t="str">
+      <c r="E68" t="str">
         <v>489,67</v>
       </c>
-      <c r="E68" t="str">
+      <c r="F68" t="str">
         <v>1606,9</v>
       </c>
-      <c r="F68" t="str">
-        <v>-</v>
-      </c>
       <c r="G68" t="str">
+        <v>-</v>
+      </c>
+      <c r="H68" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B69" t="str">
         <v>8-9</v>
       </c>
-      <c r="B69" t="str">
+      <c r="C69" t="str">
         <v>432,41</v>
       </c>
-      <c r="C69" t="str">
+      <c r="D69" t="str">
         <v>2918,7</v>
       </c>
-      <c r="D69" t="str">
+      <c r="E69" t="str">
         <v>456,00</v>
       </c>
-      <c r="E69" t="str">
+      <c r="F69" t="str">
         <v>1068,5</v>
       </c>
-      <c r="F69" t="str">
-        <v>-</v>
-      </c>
       <c r="G69" t="str">
+        <v>-</v>
+      </c>
+      <c r="H69" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B70" t="str">
         <v>9-10</v>
       </c>
-      <c r="B70" t="str">
+      <c r="C70" t="str">
         <v>355,57</v>
       </c>
-      <c r="C70" t="str">
+      <c r="D70" t="str">
         <v>3202,7</v>
       </c>
-      <c r="D70" t="str">
+      <c r="E70" t="str">
         <v>387,79</v>
       </c>
-      <c r="E70" t="str">
+      <c r="F70" t="str">
         <v>1457,7</v>
       </c>
-      <c r="F70" t="str">
+      <c r="G70" t="str">
         <v>345,00</v>
       </c>
-      <c r="G70" t="str">
+      <c r="H70" t="str">
         <v>10</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B71" t="str">
         <v>10-11</v>
       </c>
-      <c r="B71" t="str">
+      <c r="C71" t="str">
         <v>288,00</v>
       </c>
-      <c r="C71" t="str">
+      <c r="D71" t="str">
         <v>4244,9</v>
       </c>
-      <c r="D71" t="str">
+      <c r="E71" t="str">
         <v>331,19</v>
       </c>
-      <c r="E71" t="str">
+      <c r="F71" t="str">
         <v>1567,9</v>
       </c>
-      <c r="F71" t="str">
-        <v>-</v>
-      </c>
       <c r="G71" t="str">
+        <v>-</v>
+      </c>
+      <c r="H71" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B72" t="str">
         <v>11-12</v>
       </c>
-      <c r="B72" t="str">
+      <c r="C72" t="str">
         <v>263,40</v>
       </c>
-      <c r="C72" t="str">
+      <c r="D72" t="str">
         <v>4633,8</v>
       </c>
-      <c r="D72" t="str">
+      <c r="E72" t="str">
         <v>291,14</v>
       </c>
-      <c r="E72" t="str">
+      <c r="F72" t="str">
         <v>1274,8</v>
       </c>
-      <c r="F72" t="str">
-        <v>-</v>
-      </c>
       <c r="G72" t="str">
+        <v>-</v>
+      </c>
+      <c r="H72" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B73" t="str">
         <v>12-13</v>
       </c>
-      <c r="B73" t="str">
+      <c r="C73" t="str">
         <v>235,90</v>
       </c>
-      <c r="C73" t="str">
+      <c r="D73" t="str">
         <v>4504,3</v>
       </c>
-      <c r="D73" t="str">
+      <c r="E73" t="str">
         <v>275,59</v>
       </c>
-      <c r="E73" t="str">
+      <c r="F73" t="str">
         <v>1174,6</v>
       </c>
-      <c r="F73" t="str">
+      <c r="G73" t="str">
         <v>225,00</v>
       </c>
-      <c r="G73" t="str">
+      <c r="H73" t="str">
         <v>20</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B74" t="str">
         <v>13-14</v>
       </c>
-      <c r="B74" t="str">
+      <c r="C74" t="str">
         <v>241,99</v>
       </c>
-      <c r="C74" t="str">
+      <c r="D74" t="str">
         <v>4004,6</v>
       </c>
-      <c r="D74" t="str">
+      <c r="E74" t="str">
         <v>247,03</v>
       </c>
-      <c r="E74" t="str">
+      <c r="F74" t="str">
         <v>1094,2</v>
       </c>
-      <c r="F74" t="str">
+      <c r="G74" t="str">
         <v>231,31</v>
       </c>
-      <c r="G74" t="str">
+      <c r="H74" t="str">
         <v>21,1</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B75" t="str">
         <v>14-15</v>
       </c>
-      <c r="B75" t="str">
+      <c r="C75" t="str">
         <v>233,99</v>
       </c>
-      <c r="C75" t="str">
+      <c r="D75" t="str">
         <v>4052,4</v>
       </c>
-      <c r="D75" t="str">
+      <c r="E75" t="str">
         <v>226,96</v>
       </c>
-      <c r="E75" t="str">
+      <c r="F75" t="str">
         <v>1001</v>
       </c>
-      <c r="F75" t="str">
-        <v>-</v>
-      </c>
       <c r="G75" t="str">
+        <v>-</v>
+      </c>
+      <c r="H75" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B76" t="str">
         <v>15-16</v>
       </c>
-      <c r="B76" t="str">
+      <c r="C76" t="str">
         <v>295,67</v>
       </c>
-      <c r="C76" t="str">
+      <c r="D76" t="str">
         <v>3632,1</v>
       </c>
-      <c r="D76" t="str">
+      <c r="E76" t="str">
         <v>295,90</v>
       </c>
-      <c r="E76" t="str">
+      <c r="F76" t="str">
         <v>752,4</v>
       </c>
-      <c r="F76" t="str">
-        <v>-</v>
-      </c>
       <c r="G76" t="str">
+        <v>-</v>
+      </c>
+      <c r="H76" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B77" t="str">
         <v>16-17</v>
       </c>
-      <c r="B77" t="str">
+      <c r="C77" t="str">
         <v>385,69</v>
       </c>
-      <c r="C77" t="str">
+      <c r="D77" t="str">
         <v>3191,6</v>
       </c>
-      <c r="D77" t="str">
+      <c r="E77" t="str">
         <v>379,13</v>
       </c>
-      <c r="E77" t="str">
+      <c r="F77" t="str">
         <v>487,8</v>
       </c>
-      <c r="F77" t="str">
-        <v>-</v>
-      </c>
       <c r="G77" t="str">
+        <v>-</v>
+      </c>
+      <c r="H77" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B78" t="str">
         <v>17-18</v>
       </c>
-      <c r="B78" t="str">
+      <c r="C78" t="str">
         <v>444,97</v>
       </c>
-      <c r="C78" t="str">
+      <c r="D78" t="str">
         <v>3216,2</v>
       </c>
-      <c r="D78" t="str">
+      <c r="E78" t="str">
         <v>380,34</v>
       </c>
-      <c r="E78" t="str">
+      <c r="F78" t="str">
         <v>1392,1</v>
       </c>
-      <c r="F78" t="str">
-        <v>-</v>
-      </c>
       <c r="G78" t="str">
+        <v>-</v>
+      </c>
+      <c r="H78" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B79" t="str">
         <v>18-19</v>
       </c>
-      <c r="B79" t="str">
+      <c r="C79" t="str">
         <v>503,60</v>
       </c>
-      <c r="C79" t="str">
+      <c r="D79" t="str">
         <v>3604,7</v>
       </c>
-      <c r="D79" t="str">
+      <c r="E79" t="str">
         <v>460,55</v>
       </c>
-      <c r="E79" t="str">
+      <c r="F79" t="str">
         <v>2153,5</v>
       </c>
-      <c r="F79" t="str">
+      <c r="G79" t="str">
         <v>500,00</v>
       </c>
-      <c r="G79" t="str">
+      <c r="H79" t="str">
         <v>30</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B80" t="str">
         <v>19-20</v>
       </c>
-      <c r="B80" t="str">
+      <c r="C80" t="str">
         <v>612,00</v>
       </c>
-      <c r="C80" t="str">
+      <c r="D80" t="str">
         <v>4266,8</v>
       </c>
-      <c r="D80" t="str">
+      <c r="E80" t="str">
         <v>641,44</v>
       </c>
-      <c r="E80" t="str">
+      <c r="F80" t="str">
         <v>1768,4</v>
       </c>
-      <c r="F80" t="str">
+      <c r="G80" t="str">
         <v>608,80</v>
       </c>
-      <c r="G80" t="str">
+      <c r="H80" t="str">
         <v>50</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B81" t="str">
         <v>20-21</v>
       </c>
-      <c r="B81" t="str">
+      <c r="C81" t="str">
         <v>738,99</v>
       </c>
-      <c r="C81" t="str">
+      <c r="D81" t="str">
         <v>4324,7</v>
       </c>
-      <c r="D81" t="str">
+      <c r="E81" t="str">
         <v>754,06</v>
       </c>
-      <c r="E81" t="str">
+      <c r="F81" t="str">
         <v>2056,9</v>
       </c>
-      <c r="F81" t="str">
+      <c r="G81" t="str">
         <v>698,24</v>
       </c>
-      <c r="G81" t="str">
+      <c r="H81" t="str">
         <v>121</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B82" t="str">
         <v>21-22</v>
       </c>
-      <c r="B82" t="str">
+      <c r="C82" t="str">
         <v>585,00</v>
       </c>
-      <c r="C82" t="str">
+      <c r="D82" t="str">
         <v>4070</v>
       </c>
-      <c r="D82" t="str">
+      <c r="E82" t="str">
         <v>521,01</v>
       </c>
-      <c r="E82" t="str">
+      <c r="F82" t="str">
         <v>2050,3</v>
       </c>
-      <c r="F82" t="str">
+      <c r="G82" t="str">
         <v>590,00</v>
       </c>
-      <c r="G82" t="str">
+      <c r="H82" t="str">
         <v>20</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B83" t="str">
         <v>22-23</v>
       </c>
-      <c r="B83" t="str">
+      <c r="C83" t="str">
         <v>537,00</v>
       </c>
-      <c r="C83" t="str">
+      <c r="D83" t="str">
         <v>4529,6</v>
       </c>
-      <c r="D83" t="str">
+      <c r="E83" t="str">
         <v>537,60</v>
       </c>
-      <c r="E83" t="str">
+      <c r="F83" t="str">
         <v>2540</v>
       </c>
-      <c r="F83" t="str">
+      <c r="G83" t="str">
         <v>527,00</v>
       </c>
-      <c r="G83" t="str">
+      <c r="H83" t="str">
         <v>10</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B84" t="str">
         <v>23-24</v>
       </c>
-      <c r="B84" t="str">
+      <c r="C84" t="str">
         <v>450,00</v>
       </c>
-      <c r="C84" t="str">
+      <c r="D84" t="str">
         <v>3734,1</v>
       </c>
-      <c r="D84" t="str">
+      <c r="E84" t="str">
         <v>447,57</v>
       </c>
-      <c r="E84" t="str">
+      <c r="F84" t="str">
         <v>2142</v>
       </c>
-      <c r="F84" t="str">
+      <c r="G84" t="str">
         <v>440,00</v>
       </c>
-      <c r="G84" t="str">
+      <c r="H84" t="str">
         <v>10</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B85" t="str">
         <v>Min.</v>
       </c>
-      <c r="B85" t="str">
+      <c r="C85" t="str">
         <v>233,99</v>
       </c>
-      <c r="C85" t="str">
-        <v>-</v>
-      </c>
       <c r="D85" t="str">
+        <v>-</v>
+      </c>
+      <c r="E85" t="str">
         <v>226,96</v>
       </c>
-      <c r="E85" t="str">
-        <v>-</v>
-      </c>
       <c r="F85" t="str">
         <v>-</v>
       </c>
       <c r="G85" t="str">
+        <v>-</v>
+      </c>
+      <c r="H85" t="str">
         <v>-</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B86" t="str">
         <v>Maks.</v>
       </c>
-      <c r="B86" t="str">
+      <c r="C86" t="str">
         <v>738,99</v>
       </c>
-      <c r="C86" t="str">
-        <v>-</v>
-      </c>
       <c r="D86" t="str">
+        <v>-</v>
+      </c>
+      <c r="E86" t="str">
         <v>754,06</v>
       </c>
-      <c r="E86" t="str">
-        <v>-</v>
-      </c>
       <c r="F86" t="str">
         <v>-</v>
       </c>
       <c r="G86" t="str">
+        <v>-</v>
+      </c>
+      <c r="H86" t="str">
         <v>-</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
+        <v>31-07-2024</v>
+      </c>
+      <c r="B87" t="str">
         <v>Suma</v>
       </c>
-      <c r="B87" t="str">
+      <c r="C87" t="str">
         <v/>
       </c>
-      <c r="C87" t="str">
+      <c r="D87" t="str">
         <v>87 482</v>
       </c>
-      <c r="D87" t="str">
+      <c r="E87" t="str">
         <v/>
       </c>
-      <c r="E87" t="str">
+      <c r="F87" t="str">
         <v>42 221,8</v>
       </c>
-      <c r="F87" t="str">
+      <c r="G87" t="str">
         <v/>
       </c>
-      <c r="G87" t="str">
+      <c r="H87" t="str">
         <v>349,2</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B88" t="str">
         <v/>
       </c>
-      <c r="B88" t="str">
+      <c r="C88" t="str">
         <v>FIXING I</v>
       </c>
-      <c r="C88" t="str">
+      <c r="D88" t="str">
         <v>FIXING II</v>
       </c>
-      <c r="D88" t="str">
+      <c r="E88" t="str">
         <v>Notowania ciągłe</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B89" t="str">
         <v>Czas</v>
       </c>
-      <c r="B89" t="str">
+      <c r="C89" t="str">
         <v>Kurs (PLN/MWh)</v>
       </c>
-      <c r="C89" t="str">
+      <c r="D89" t="str">
         <v>Wolumen (MWh)</v>
       </c>
-      <c r="D89" t="str">
+      <c r="E89" t="str">
         <v>Kurs (PLN/MWh)</v>
       </c>
-      <c r="E89" t="str">
+      <c r="F89" t="str">
         <v>Wolumen (MWh)</v>
       </c>
-      <c r="F89" t="str">
+      <c r="G89" t="str">
         <v>Kurs (PLN/MWh)</v>
       </c>
-      <c r="G89" t="str">
+      <c r="H89" t="str">
         <v>Wolumen (MWh)</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B90" t="str">
         <v>0-1</v>
       </c>
-      <c r="B90" t="str">
+      <c r="C90" t="str">
         <v>465,00</v>
       </c>
-      <c r="C90" t="str">
+      <c r="D90" t="str">
         <v>3086,1</v>
       </c>
-      <c r="D90" t="str">
+      <c r="E90" t="str">
         <v>429,92</v>
       </c>
-      <c r="E90" t="str">
+      <c r="F90" t="str">
         <v>2058,9</v>
       </c>
-      <c r="F90" t="str">
+      <c r="G90" t="str">
         <v>455,00</v>
       </c>
-      <c r="G90" t="str">
+      <c r="H90" t="str">
         <v>20</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B91" t="str">
         <v>1-2</v>
       </c>
-      <c r="B91" t="str">
+      <c r="C91" t="str">
         <v>400,00</v>
       </c>
-      <c r="C91" t="str">
+      <c r="D91" t="str">
         <v>2943,5</v>
       </c>
-      <c r="D91" t="str">
+      <c r="E91" t="str">
         <v>385,88</v>
       </c>
-      <c r="E91" t="str">
+      <c r="F91" t="str">
         <v>1456,5</v>
       </c>
-      <c r="F91" t="str">
-        <v>-</v>
-      </c>
       <c r="G91" t="str">
+        <v>-</v>
+      </c>
+      <c r="H91" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B92" t="str">
         <v>2-3</v>
       </c>
-      <c r="B92" t="str">
+      <c r="C92" t="str">
         <v>392,00</v>
       </c>
-      <c r="C92" t="str">
+      <c r="D92" t="str">
         <v>2758,5</v>
       </c>
-      <c r="D92" t="str">
+      <c r="E92" t="str">
         <v>385,69</v>
       </c>
-      <c r="E92" t="str">
+      <c r="F92" t="str">
         <v>1497,3</v>
       </c>
-      <c r="F92" t="str">
-        <v>-</v>
-      </c>
       <c r="G92" t="str">
+        <v>-</v>
+      </c>
+      <c r="H92" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B93" t="str">
         <v>3-4</v>
       </c>
-      <c r="B93" t="str">
+      <c r="C93" t="str">
         <v>388,00</v>
       </c>
-      <c r="C93" t="str">
+      <c r="D93" t="str">
         <v>2813,8</v>
       </c>
-      <c r="D93" t="str">
+      <c r="E93" t="str">
         <v>387,52</v>
       </c>
-      <c r="E93" t="str">
+      <c r="F93" t="str">
         <v>1859,4</v>
       </c>
-      <c r="F93" t="str">
-        <v>-</v>
-      </c>
       <c r="G93" t="str">
+        <v>-</v>
+      </c>
+      <c r="H93" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B94" t="str">
         <v>4-5</v>
       </c>
-      <c r="B94" t="str">
+      <c r="C94" t="str">
         <v>390,00</v>
       </c>
-      <c r="C94" t="str">
+      <c r="D94" t="str">
         <v>3016,1</v>
       </c>
-      <c r="D94" t="str">
+      <c r="E94" t="str">
         <v>385,69</v>
       </c>
-      <c r="E94" t="str">
+      <c r="F94" t="str">
         <v>1854,9</v>
       </c>
-      <c r="F94" t="str">
-        <v>-</v>
-      </c>
       <c r="G94" t="str">
+        <v>-</v>
+      </c>
+      <c r="H94" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B95" t="str">
         <v>5-6</v>
       </c>
-      <c r="B95" t="str">
+      <c r="C95" t="str">
         <v>431,28</v>
       </c>
-      <c r="C95" t="str">
+      <c r="D95" t="str">
         <v>3273,4</v>
       </c>
-      <c r="D95" t="str">
+      <c r="E95" t="str">
         <v>387,92</v>
       </c>
-      <c r="E95" t="str">
+      <c r="F95" t="str">
         <v>1578,2</v>
       </c>
-      <c r="F95" t="str">
-        <v>-</v>
-      </c>
       <c r="G95" t="str">
+        <v>-</v>
+      </c>
+      <c r="H95" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B96" t="str">
         <v>6-7</v>
       </c>
-      <c r="B96" t="str">
+      <c r="C96" t="str">
         <v>542,00</v>
       </c>
-      <c r="C96" t="str">
+      <c r="D96" t="str">
         <v>3581,2</v>
       </c>
-      <c r="D96" t="str">
+      <c r="E96" t="str">
         <v>476,66</v>
       </c>
-      <c r="E96" t="str">
+      <c r="F96" t="str">
         <v>1899,5</v>
       </c>
-      <c r="F96" t="str">
-        <v>-</v>
-      </c>
       <c r="G96" t="str">
+        <v>-</v>
+      </c>
+      <c r="H96" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B97" t="str">
         <v>7-8</v>
       </c>
-      <c r="B97" t="str">
+      <c r="C97" t="str">
         <v>540,00</v>
       </c>
-      <c r="C97" t="str">
+      <c r="D97" t="str">
         <v>3027,6</v>
       </c>
-      <c r="D97" t="str">
+      <c r="E97" t="str">
         <v>520,50</v>
       </c>
-      <c r="E97" t="str">
+      <c r="F97" t="str">
         <v>1580,2</v>
       </c>
-      <c r="F97" t="str">
-        <v>-</v>
-      </c>
       <c r="G97" t="str">
+        <v>-</v>
+      </c>
+      <c r="H97" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B98" t="str">
         <v>8-9</v>
       </c>
-      <c r="B98" t="str">
+      <c r="C98" t="str">
         <v>488,50</v>
       </c>
-      <c r="C98" t="str">
+      <c r="D98" t="str">
         <v>2854,3</v>
       </c>
-      <c r="D98" t="str">
+      <c r="E98" t="str">
         <v>486,19</v>
       </c>
-      <c r="E98" t="str">
+      <c r="F98" t="str">
         <v>879,8</v>
       </c>
-      <c r="F98" t="str">
+      <c r="G98" t="str">
         <v>488,45</v>
       </c>
-      <c r="G98" t="str">
+      <c r="H98" t="str">
         <v>41</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B99" t="str">
         <v>9-10</v>
       </c>
-      <c r="B99" t="str">
+      <c r="C99" t="str">
         <v>450,00</v>
       </c>
-      <c r="C99" t="str">
+      <c r="D99" t="str">
         <v>2832,4</v>
       </c>
-      <c r="D99" t="str">
+      <c r="E99" t="str">
         <v>448,80</v>
       </c>
-      <c r="E99" t="str">
+      <c r="F99" t="str">
         <v>876,3</v>
       </c>
-      <c r="F99" t="str">
+      <c r="G99" t="str">
         <v>450,00</v>
       </c>
-      <c r="G99" t="str">
+      <c r="H99" t="str">
         <v>15</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B100" t="str">
         <v>10-11</v>
       </c>
-      <c r="B100" t="str">
+      <c r="C100" t="str">
         <v>404,00</v>
       </c>
-      <c r="C100" t="str">
+      <c r="D100" t="str">
         <v>3020,4</v>
       </c>
-      <c r="D100" t="str">
+      <c r="E100" t="str">
         <v>385,42</v>
       </c>
-      <c r="E100" t="str">
+      <c r="F100" t="str">
         <v>913,9</v>
       </c>
-      <c r="F100" t="str">
+      <c r="G100" t="str">
         <v>404,00</v>
       </c>
-      <c r="G100" t="str">
+      <c r="H100" t="str">
         <v>15</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B101" t="str">
         <v>11-12</v>
       </c>
-      <c r="B101" t="str">
+      <c r="C101" t="str">
         <v>390,34</v>
       </c>
-      <c r="C101" t="str">
+      <c r="D101" t="str">
         <v>3327,3</v>
       </c>
-      <c r="D101" t="str">
+      <c r="E101" t="str">
         <v>344,07</v>
       </c>
-      <c r="E101" t="str">
+      <c r="F101" t="str">
         <v>975,7</v>
       </c>
-      <c r="F101" t="str">
+      <c r="G101" t="str">
         <v>390,34</v>
       </c>
-      <c r="G101" t="str">
+      <c r="H101" t="str">
         <v>9</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B102" t="str">
         <v>12-13</v>
       </c>
-      <c r="B102" t="str">
+      <c r="C102" t="str">
         <v>387,59</v>
       </c>
-      <c r="C102" t="str">
+      <c r="D102" t="str">
         <v>3357,9</v>
       </c>
-      <c r="D102" t="str">
+      <c r="E102" t="str">
         <v>354,72</v>
       </c>
-      <c r="E102" t="str">
+      <c r="F102" t="str">
         <v>836,5</v>
       </c>
-      <c r="F102" t="str">
+      <c r="G102" t="str">
         <v>387,59</v>
       </c>
-      <c r="G102" t="str">
+      <c r="H102" t="str">
         <v>6</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B103" t="str">
         <v>13-14</v>
       </c>
-      <c r="B103" t="str">
+      <c r="C103" t="str">
         <v>394,00</v>
       </c>
-      <c r="C103" t="str">
+      <c r="D103" t="str">
         <v>3262,1</v>
       </c>
-      <c r="D103" t="str">
+      <c r="E103" t="str">
         <v>368,09</v>
       </c>
-      <c r="E103" t="str">
+      <c r="F103" t="str">
         <v>783,7</v>
       </c>
-      <c r="F103" t="str">
-        <v>-</v>
-      </c>
       <c r="G103" t="str">
+        <v>-</v>
+      </c>
+      <c r="H103" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B104" t="str">
         <v>14-15</v>
       </c>
-      <c r="B104" t="str">
+      <c r="C104" t="str">
         <v>406,00</v>
       </c>
-      <c r="C104" t="str">
+      <c r="D104" t="str">
         <v>3301,9</v>
       </c>
-      <c r="D104" t="str">
+      <c r="E104" t="str">
         <v>405,43</v>
       </c>
-      <c r="E104" t="str">
+      <c r="F104" t="str">
         <v>618</v>
       </c>
-      <c r="F104" t="str">
+      <c r="G104" t="str">
         <v>406,00</v>
       </c>
-      <c r="G104" t="str">
+      <c r="H104" t="str">
         <v>12,1</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B105" t="str">
         <v>15-16</v>
       </c>
-      <c r="B105" t="str">
+      <c r="C105" t="str">
         <v>482,86</v>
       </c>
-      <c r="C105" t="str">
+      <c r="D105" t="str">
         <v>3687</v>
       </c>
-      <c r="D105" t="str">
+      <c r="E105" t="str">
         <v>484,29</v>
       </c>
-      <c r="E105" t="str">
+      <c r="F105" t="str">
         <v>682,7</v>
       </c>
-      <c r="F105" t="str">
+      <c r="G105" t="str">
         <v>482,86</v>
       </c>
-      <c r="G105" t="str">
+      <c r="H105" t="str">
         <v>19,7</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B106" t="str">
         <v>16-17</v>
       </c>
-      <c r="B106" t="str">
+      <c r="C106" t="str">
         <v>482,86</v>
       </c>
-      <c r="C106" t="str">
+      <c r="D106" t="str">
         <v>4076,7</v>
       </c>
-      <c r="D106" t="str">
+      <c r="E106" t="str">
         <v>496,07</v>
       </c>
-      <c r="E106" t="str">
+      <c r="F106" t="str">
         <v>1381,1</v>
       </c>
-      <c r="F106" t="str">
-        <v>-</v>
-      </c>
       <c r="G106" t="str">
+        <v>-</v>
+      </c>
+      <c r="H106" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B107" t="str">
         <v>17-18</v>
       </c>
-      <c r="B107" t="str">
+      <c r="C107" t="str">
         <v>469,00</v>
       </c>
-      <c r="C107" t="str">
+      <c r="D107" t="str">
         <v>4080,3</v>
       </c>
-      <c r="D107" t="str">
+      <c r="E107" t="str">
         <v>490,81</v>
       </c>
-      <c r="E107" t="str">
+      <c r="F107" t="str">
         <v>2231,3</v>
       </c>
-      <c r="F107" t="str">
+      <c r="G107" t="str">
         <v>469,00</v>
       </c>
-      <c r="G107" t="str">
+      <c r="H107" t="str">
         <v>43</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B108" t="str">
         <v>18-19</v>
       </c>
-      <c r="B108" t="str">
+      <c r="C108" t="str">
         <v>549,00</v>
       </c>
-      <c r="C108" t="str">
+      <c r="D108" t="str">
         <v>3853,5</v>
       </c>
-      <c r="D108" t="str">
+      <c r="E108" t="str">
         <v>550,60</v>
       </c>
-      <c r="E108" t="str">
+      <c r="F108" t="str">
         <v>2442,6</v>
       </c>
-      <c r="F108" t="str">
+      <c r="G108" t="str">
         <v>545,00</v>
       </c>
-      <c r="G108" t="str">
+      <c r="H108" t="str">
         <v>30</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B109" t="str">
         <v>19-20</v>
       </c>
-      <c r="B109" t="str">
+      <c r="C109" t="str">
         <v>600,00</v>
       </c>
-      <c r="C109" t="str">
+      <c r="D109" t="str">
         <v>4099,8</v>
       </c>
-      <c r="D109" t="str">
+      <c r="E109" t="str">
         <v>565,57</v>
       </c>
-      <c r="E109" t="str">
+      <c r="F109" t="str">
         <v>2106,3</v>
       </c>
-      <c r="F109" t="str">
+      <c r="G109" t="str">
         <v>590,00</v>
       </c>
-      <c r="G109" t="str">
+      <c r="H109" t="str">
         <v>5</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B110" t="str">
         <v>20-21</v>
       </c>
-      <c r="B110" t="str">
+      <c r="C110" t="str">
         <v>670,00</v>
       </c>
-      <c r="C110" t="str">
+      <c r="D110" t="str">
         <v>3956,3</v>
       </c>
-      <c r="D110" t="str">
+      <c r="E110" t="str">
         <v>674,30</v>
       </c>
-      <c r="E110" t="str">
+      <c r="F110" t="str">
         <v>1721,6</v>
       </c>
-      <c r="F110" t="str">
+      <c r="G110" t="str">
         <v>670,51</v>
       </c>
-      <c r="G110" t="str">
+      <c r="H110" t="str">
         <v>5</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B111" t="str">
         <v>21-22</v>
       </c>
-      <c r="B111" t="str">
+      <c r="C111" t="str">
         <v>553,90</v>
       </c>
-      <c r="C111" t="str">
+      <c r="D111" t="str">
         <v>3775,1</v>
       </c>
-      <c r="D111" t="str">
+      <c r="E111" t="str">
         <v>553,22</v>
       </c>
-      <c r="E111" t="str">
+      <c r="F111" t="str">
         <v>1724,7</v>
       </c>
-      <c r="F111" t="str">
+      <c r="G111" t="str">
         <v>567,57</v>
       </c>
-      <c r="G111" t="str">
+      <c r="H111" t="str">
         <v>33</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B112" t="str">
         <v>22-23</v>
       </c>
-      <c r="B112" t="str">
+      <c r="C112" t="str">
         <v>513,70</v>
       </c>
-      <c r="C112" t="str">
+      <c r="D112" t="str">
         <v>4049,7</v>
       </c>
-      <c r="D112" t="str">
+      <c r="E112" t="str">
         <v>495,48</v>
       </c>
-      <c r="E112" t="str">
+      <c r="F112" t="str">
         <v>2430,9</v>
       </c>
-      <c r="F112" t="str">
-        <v>-</v>
-      </c>
       <c r="G112" t="str">
+        <v>-</v>
+      </c>
+      <c r="H112" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B113" t="str">
         <v>23-24</v>
       </c>
-      <c r="B113" t="str">
+      <c r="C113" t="str">
         <v>449,00</v>
       </c>
-      <c r="C113" t="str">
+      <c r="D113" t="str">
         <v>3402,8</v>
       </c>
-      <c r="D113" t="str">
+      <c r="E113" t="str">
         <v>435,23</v>
       </c>
-      <c r="E113" t="str">
+      <c r="F113" t="str">
         <v>1887</v>
       </c>
-      <c r="F113" t="str">
-        <v>-</v>
-      </c>
       <c r="G113" t="str">
+        <v>-</v>
+      </c>
+      <c r="H113" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B114" t="str">
         <v>Min.</v>
       </c>
-      <c r="B114" t="str">
+      <c r="C114" t="str">
         <v>387,59</v>
       </c>
-      <c r="C114" t="str">
-        <v>-</v>
-      </c>
       <c r="D114" t="str">
+        <v>-</v>
+      </c>
+      <c r="E114" t="str">
         <v>344,07</v>
       </c>
-      <c r="E114" t="str">
-        <v>-</v>
-      </c>
       <c r="F114" t="str">
+        <v>-</v>
+      </c>
+      <c r="G114" t="str">
         <v>387,59</v>
       </c>
-      <c r="G114" t="str">
+      <c r="H114" t="str">
         <v>-</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B115" t="str">
         <v>Maks.</v>
       </c>
-      <c r="B115" t="str">
+      <c r="C115" t="str">
         <v>670,00</v>
       </c>
-      <c r="C115" t="str">
-        <v>-</v>
-      </c>
       <c r="D115" t="str">
+        <v>-</v>
+      </c>
+      <c r="E115" t="str">
         <v>674,30</v>
       </c>
-      <c r="E115" t="str">
-        <v>-</v>
-      </c>
       <c r="F115" t="str">
+        <v>-</v>
+      </c>
+      <c r="G115" t="str">
         <v>670,51</v>
       </c>
-      <c r="G115" t="str">
+      <c r="H115" t="str">
         <v>-</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
+        <v>01-08-2024</v>
+      </c>
+      <c r="B116" t="str">
         <v>Suma</v>
       </c>
-      <c r="B116" t="str">
+      <c r="C116" t="str">
         <v/>
       </c>
-      <c r="C116" t="str">
+      <c r="D116" t="str">
         <v>81 437,7</v>
       </c>
-      <c r="D116" t="str">
+      <c r="E116" t="str">
         <v/>
       </c>
-      <c r="E116" t="str">
+      <c r="F116" t="str">
         <v>36 277</v>
       </c>
-      <c r="F116" t="str">
+      <c r="G116" t="str">
         <v/>
       </c>
-      <c r="G116" t="str">
+      <c r="H116" t="str">
         <v>253,8</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B117" t="str">
         <v/>
       </c>
-      <c r="B117" t="str">
+      <c r="C117" t="str">
         <v>FIXING I</v>
       </c>
-      <c r="C117" t="str">
+      <c r="D117" t="str">
         <v>FIXING II</v>
       </c>
-      <c r="D117" t="str">
+      <c r="E117" t="str">
         <v>Notowania ciągłe</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B118" t="str">
         <v>Czas</v>
       </c>
-      <c r="B118" t="str">
+      <c r="C118" t="str">
         <v>Kurs (PLN/MWh)</v>
       </c>
-      <c r="C118" t="str">
+      <c r="D118" t="str">
         <v>Wolumen (MWh)</v>
       </c>
-      <c r="D118" t="str">
+      <c r="E118" t="str">
         <v>Kurs (PLN/MWh)</v>
       </c>
-      <c r="E118" t="str">
+      <c r="F118" t="str">
         <v>Wolumen (MWh)</v>
       </c>
-      <c r="F118" t="str">
+      <c r="G118" t="str">
         <v>Kurs (PLN/MWh)</v>
       </c>
-      <c r="G118" t="str">
+      <c r="H118" t="str">
         <v>Wolumen (MWh)</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B119" t="str">
         <v>0-1</v>
       </c>
-      <c r="B119" t="str">
+      <c r="C119" t="str">
         <v>490,00</v>
       </c>
-      <c r="C119" t="str">
+      <c r="D119" t="str">
         <v>3019,5</v>
       </c>
-      <c r="D119" t="str">
+      <c r="E119" t="str">
         <v>490,60</v>
       </c>
-      <c r="E119" t="str">
+      <c r="F119" t="str">
         <v>1973,1</v>
       </c>
-      <c r="F119" t="str">
+      <c r="G119" t="str">
         <v>488,00</v>
       </c>
-      <c r="G119" t="str">
+      <c r="H119" t="str">
         <v>1,5</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B120" t="str">
         <v>1-2</v>
       </c>
-      <c r="B120" t="str">
+      <c r="C120" t="str">
         <v>450,00</v>
       </c>
-      <c r="C120" t="str">
+      <c r="D120" t="str">
         <v>2661,6</v>
       </c>
-      <c r="D120" t="str">
+      <c r="E120" t="str">
         <v>488,64</v>
       </c>
-      <c r="E120" t="str">
+      <c r="F120" t="str">
         <v>1632,2</v>
       </c>
-      <c r="F120" t="str">
+      <c r="G120" t="str">
         <v>447,00</v>
       </c>
-      <c r="G120" t="str">
+      <c r="H120" t="str">
         <v>10</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B121" t="str">
         <v>2-3</v>
       </c>
-      <c r="B121" t="str">
+      <c r="C121" t="str">
         <v>424,41</v>
       </c>
-      <c r="C121" t="str">
+      <c r="D121" t="str">
         <v>2467,2</v>
       </c>
-      <c r="D121" t="str">
+      <c r="E121" t="str">
         <v>474,92</v>
       </c>
-      <c r="E121" t="str">
+      <c r="F121" t="str">
         <v>1515,4</v>
       </c>
-      <c r="F121" t="str">
-        <v>-</v>
-      </c>
       <c r="G121" t="str">
+        <v>-</v>
+      </c>
+      <c r="H121" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B122" t="str">
         <v>3-4</v>
       </c>
-      <c r="B122" t="str">
+      <c r="C122" t="str">
         <v>436,90</v>
       </c>
-      <c r="C122" t="str">
+      <c r="D122" t="str">
         <v>2551,9</v>
       </c>
-      <c r="D122" t="str">
+      <c r="E122" t="str">
         <v>481,66</v>
       </c>
-      <c r="E122" t="str">
+      <c r="F122" t="str">
         <v>1360,2</v>
       </c>
-      <c r="F122" t="str">
-        <v>-</v>
-      </c>
       <c r="G122" t="str">
+        <v>-</v>
+      </c>
+      <c r="H122" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B123" t="str">
         <v>4-5</v>
       </c>
-      <c r="B123" t="str">
+      <c r="C123" t="str">
         <v>428,00</v>
       </c>
-      <c r="C123" t="str">
+      <c r="D123" t="str">
         <v>2586,7</v>
       </c>
-      <c r="D123" t="str">
+      <c r="E123" t="str">
         <v>481,47</v>
       </c>
-      <c r="E123" t="str">
+      <c r="F123" t="str">
         <v>1293,1</v>
       </c>
-      <c r="F123" t="str">
-        <v>-</v>
-      </c>
       <c r="G123" t="str">
+        <v>-</v>
+      </c>
+      <c r="H123" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B124" t="str">
         <v>5-6</v>
       </c>
-      <c r="B124" t="str">
+      <c r="C124" t="str">
         <v>447,91</v>
       </c>
-      <c r="C124" t="str">
+      <c r="D124" t="str">
         <v>2458,7</v>
       </c>
-      <c r="D124" t="str">
+      <c r="E124" t="str">
         <v>487,59</v>
       </c>
-      <c r="E124" t="str">
+      <c r="F124" t="str">
         <v>1202,2</v>
       </c>
-      <c r="F124" t="str">
+      <c r="G124" t="str">
         <v>445,92</v>
       </c>
-      <c r="G124" t="str">
+      <c r="H124" t="str">
         <v>34,3</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B125" t="str">
         <v>6-7</v>
       </c>
-      <c r="B125" t="str">
+      <c r="C125" t="str">
         <v>480,00</v>
       </c>
-      <c r="C125" t="str">
+      <c r="D125" t="str">
         <v>2458,6</v>
       </c>
-      <c r="D125" t="str">
+      <c r="E125" t="str">
         <v>485,88</v>
       </c>
-      <c r="E125" t="str">
+      <c r="F125" t="str">
         <v>1354,6</v>
       </c>
-      <c r="F125" t="str">
+      <c r="G125" t="str">
         <v>480,00</v>
       </c>
-      <c r="G125" t="str">
+      <c r="H125" t="str">
         <v>25,5</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B126" t="str">
         <v>7-8</v>
       </c>
-      <c r="B126" t="str">
+      <c r="C126" t="str">
         <v>488,68</v>
       </c>
-      <c r="C126" t="str">
+      <c r="D126" t="str">
         <v>2647,6</v>
       </c>
-      <c r="D126" t="str">
+      <c r="E126" t="str">
         <v>505,00</v>
       </c>
-      <c r="E126" t="str">
+      <c r="F126" t="str">
         <v>1317,3</v>
       </c>
-      <c r="F126" t="str">
+      <c r="G126" t="str">
         <v>488,68</v>
       </c>
-      <c r="G126" t="str">
+      <c r="H126" t="str">
         <v>14,7</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B127" t="str">
         <v>8-9</v>
       </c>
-      <c r="B127" t="str">
+      <c r="C127" t="str">
         <v>524,27</v>
       </c>
-      <c r="C127" t="str">
+      <c r="D127" t="str">
         <v>2835,2</v>
       </c>
-      <c r="D127" t="str">
+      <c r="E127" t="str">
         <v>533,73</v>
       </c>
-      <c r="E127" t="str">
+      <c r="F127" t="str">
         <v>894</v>
       </c>
-      <c r="F127" t="str">
+      <c r="G127" t="str">
         <v>524,27</v>
       </c>
-      <c r="G127" t="str">
+      <c r="H127" t="str">
         <v>2,4</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B128" t="str">
         <v>9-10</v>
       </c>
-      <c r="B128" t="str">
+      <c r="C128" t="str">
         <v>406,00</v>
       </c>
-      <c r="C128" t="str">
+      <c r="D128" t="str">
         <v>3062,2</v>
       </c>
-      <c r="D128" t="str">
+      <c r="E128" t="str">
         <v>430,75</v>
       </c>
-      <c r="E128" t="str">
+      <c r="F128" t="str">
         <v>998,9</v>
       </c>
-      <c r="F128" t="str">
-        <v>-</v>
-      </c>
       <c r="G128" t="str">
+        <v>-</v>
+      </c>
+      <c r="H128" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B129" t="str">
         <v>10-11</v>
       </c>
-      <c r="B129" t="str">
+      <c r="C129" t="str">
         <v>388,80</v>
       </c>
-      <c r="C129" t="str">
+      <c r="D129" t="str">
         <v>3177,7</v>
       </c>
-      <c r="D129" t="str">
+      <c r="E129" t="str">
         <v>390,11</v>
       </c>
-      <c r="E129" t="str">
+      <c r="F129" t="str">
         <v>829,8</v>
       </c>
-      <c r="F129" t="str">
-        <v>-</v>
-      </c>
       <c r="G129" t="str">
+        <v>-</v>
+      </c>
+      <c r="H129" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B130" t="str">
         <v>11-12</v>
       </c>
-      <c r="B130" t="str">
+      <c r="C130" t="str">
         <v>377,76</v>
       </c>
-      <c r="C130" t="str">
+      <c r="D130" t="str">
         <v>3483,6</v>
       </c>
-      <c r="D130" t="str">
+      <c r="E130" t="str">
         <v>388,26</v>
       </c>
-      <c r="E130" t="str">
+      <c r="F130" t="str">
         <v>747</v>
       </c>
-      <c r="F130" t="str">
+      <c r="G130" t="str">
         <v>375,00</v>
       </c>
-      <c r="G130" t="str">
+      <c r="H130" t="str">
         <v>11</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B131" t="str">
         <v>12-13</v>
       </c>
-      <c r="B131" t="str">
+      <c r="C131" t="str">
         <v>361,40</v>
       </c>
-      <c r="C131" t="str">
+      <c r="D131" t="str">
         <v>3870,2</v>
       </c>
-      <c r="D131" t="str">
+      <c r="E131" t="str">
         <v>379,29</v>
       </c>
-      <c r="E131" t="str">
+      <c r="F131" t="str">
         <v>844,5</v>
       </c>
-      <c r="F131" t="str">
-        <v>-</v>
-      </c>
       <c r="G131" t="str">
+        <v>-</v>
+      </c>
+      <c r="H131" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B132" t="str">
         <v>13-14</v>
       </c>
-      <c r="B132" t="str">
+      <c r="C132" t="str">
         <v>326,70</v>
       </c>
-      <c r="C132" t="str">
+      <c r="D132" t="str">
         <v>3254,2</v>
       </c>
-      <c r="D132" t="str">
+      <c r="E132" t="str">
         <v>301,05</v>
       </c>
-      <c r="E132" t="str">
+      <c r="F132" t="str">
         <v>991,1</v>
       </c>
-      <c r="F132" t="str">
-        <v>-</v>
-      </c>
       <c r="G132" t="str">
+        <v>-</v>
+      </c>
+      <c r="H132" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B133" t="str">
         <v>14-15</v>
       </c>
-      <c r="B133" t="str">
+      <c r="C133" t="str">
         <v>300,00</v>
       </c>
-      <c r="C133" t="str">
+      <c r="D133" t="str">
         <v>3199,1</v>
       </c>
-      <c r="D133" t="str">
+      <c r="E133" t="str">
         <v>290,79</v>
       </c>
-      <c r="E133" t="str">
+      <c r="F133" t="str">
         <v>895,5</v>
       </c>
-      <c r="F133" t="str">
+      <c r="G133" t="str">
         <v>297,00</v>
       </c>
-      <c r="G133" t="str">
+      <c r="H133" t="str">
         <v>30</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B134" t="str">
         <v>15-16</v>
       </c>
-      <c r="B134" t="str">
+      <c r="C134" t="str">
         <v>340,00</v>
       </c>
-      <c r="C134" t="str">
+      <c r="D134" t="str">
         <v>2942,2</v>
       </c>
-      <c r="D134" t="str">
+      <c r="E134" t="str">
         <v>323,78</v>
       </c>
-      <c r="E134" t="str">
+      <c r="F134" t="str">
         <v>761,8</v>
       </c>
-      <c r="F134" t="str">
+      <c r="G134" t="str">
         <v>337,00</v>
       </c>
-      <c r="G134" t="str">
+      <c r="H134" t="str">
         <v>20,9</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B135" t="str">
         <v>16-17</v>
       </c>
-      <c r="B135" t="str">
+      <c r="C135" t="str">
         <v>399,99</v>
       </c>
-      <c r="C135" t="str">
+      <c r="D135" t="str">
         <v>3062,5</v>
       </c>
-      <c r="D135" t="str">
+      <c r="E135" t="str">
         <v>399,33</v>
       </c>
-      <c r="E135" t="str">
+      <c r="F135" t="str">
         <v>869,2</v>
       </c>
-      <c r="F135" t="str">
-        <v>-</v>
-      </c>
       <c r="G135" t="str">
+        <v>-</v>
+      </c>
+      <c r="H135" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B136" t="str">
         <v>17-18</v>
       </c>
-      <c r="B136" t="str">
+      <c r="C136" t="str">
         <v>492,90</v>
       </c>
-      <c r="C136" t="str">
+      <c r="D136" t="str">
         <v>3179,4</v>
       </c>
-      <c r="D136" t="str">
+      <c r="E136" t="str">
         <v>493,64</v>
       </c>
-      <c r="E136" t="str">
+      <c r="F136" t="str">
         <v>866,5</v>
       </c>
-      <c r="F136" t="str">
+      <c r="G136" t="str">
         <v>483,00</v>
       </c>
-      <c r="G136" t="str">
+      <c r="H136" t="str">
         <v>15</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B137" t="str">
         <v>18-19</v>
       </c>
-      <c r="B137" t="str">
+      <c r="C137" t="str">
         <v>490,00</v>
       </c>
-      <c r="C137" t="str">
+      <c r="D137" t="str">
         <v>3529,5</v>
       </c>
-      <c r="D137" t="str">
+      <c r="E137" t="str">
         <v>490,55</v>
       </c>
-      <c r="E137" t="str">
+      <c r="F137" t="str">
         <v>2271,5</v>
       </c>
-      <c r="F137" t="str">
-        <v>-</v>
-      </c>
       <c r="G137" t="str">
+        <v>-</v>
+      </c>
+      <c r="H137" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B138" t="str">
         <v>19-20</v>
       </c>
-      <c r="B138" t="str">
+      <c r="C138" t="str">
         <v>560,00</v>
       </c>
-      <c r="C138" t="str">
+      <c r="D138" t="str">
         <v>3985,3</v>
       </c>
-      <c r="D138" t="str">
+      <c r="E138" t="str">
         <v>489,60</v>
       </c>
-      <c r="E138" t="str">
+      <c r="F138" t="str">
         <v>2538,9</v>
       </c>
-      <c r="F138" t="str">
+      <c r="G138" t="str">
         <v>559,60</v>
       </c>
-      <c r="G138" t="str">
+      <c r="H138" t="str">
         <v>55</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B139" t="str">
         <v>20-21</v>
       </c>
-      <c r="B139" t="str">
+      <c r="C139" t="str">
         <v>600,00</v>
       </c>
-      <c r="C139" t="str">
+      <c r="D139" t="str">
         <v>4232</v>
       </c>
-      <c r="D139" t="str">
+      <c r="E139" t="str">
         <v>548,54</v>
       </c>
-      <c r="E139" t="str">
+      <c r="F139" t="str">
         <v>2451,3</v>
       </c>
-      <c r="F139" t="str">
+      <c r="G139" t="str">
         <v>589,14</v>
       </c>
-      <c r="G139" t="str">
+      <c r="H139" t="str">
         <v>35</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B140" t="str">
         <v>21-22</v>
       </c>
-      <c r="B140" t="str">
+      <c r="C140" t="str">
         <v>586,61</v>
       </c>
-      <c r="C140" t="str">
+      <c r="D140" t="str">
         <v>4061,9</v>
       </c>
-      <c r="D140" t="str">
+      <c r="E140" t="str">
         <v>520,53</v>
       </c>
-      <c r="E140" t="str">
+      <c r="F140" t="str">
         <v>2508,4</v>
       </c>
-      <c r="F140" t="str">
+      <c r="G140" t="str">
         <v>568,67</v>
       </c>
-      <c r="G140" t="str">
+      <c r="H140" t="str">
         <v>15</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B141" t="str">
         <v>22-23</v>
       </c>
-      <c r="B141" t="str">
+      <c r="C141" t="str">
         <v>514,80</v>
       </c>
-      <c r="C141" t="str">
+      <c r="D141" t="str">
         <v>3420,9</v>
       </c>
-      <c r="D141" t="str">
+      <c r="E141" t="str">
         <v>481,00</v>
       </c>
-      <c r="E141" t="str">
+      <c r="F141" t="str">
         <v>2467,5</v>
       </c>
-      <c r="F141" t="str">
-        <v>-</v>
-      </c>
       <c r="G141" t="str">
+        <v>-</v>
+      </c>
+      <c r="H141" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B142" t="str">
         <v>23-24</v>
       </c>
-      <c r="B142" t="str">
+      <c r="C142" t="str">
         <v>441,87</v>
       </c>
-      <c r="C142" t="str">
+      <c r="D142" t="str">
         <v>2781,6</v>
       </c>
-      <c r="D142" t="str">
+      <c r="E142" t="str">
         <v>420,40</v>
       </c>
-      <c r="E142" t="str">
+      <c r="F142" t="str">
         <v>2133,2</v>
       </c>
-      <c r="F142" t="str">
-        <v>-</v>
-      </c>
       <c r="G142" t="str">
+        <v>-</v>
+      </c>
+      <c r="H142" t="str">
         <v>0</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B143" t="str">
         <v>Min.</v>
       </c>
-      <c r="B143" t="str">
+      <c r="C143" t="str">
         <v>300,00</v>
       </c>
-      <c r="C143" t="str">
-        <v>-</v>
-      </c>
       <c r="D143" t="str">
+        <v>-</v>
+      </c>
+      <c r="E143" t="str">
         <v>290,79</v>
       </c>
-      <c r="E143" t="str">
-        <v>-</v>
-      </c>
       <c r="F143" t="str">
+        <v>-</v>
+      </c>
+      <c r="G143" t="str">
         <v>297,00</v>
       </c>
-      <c r="G143" t="str">
+      <c r="H143" t="str">
         <v>-</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B144" t="str">
         <v>Maks.</v>
       </c>
-      <c r="B144" t="str">
+      <c r="C144" t="str">
         <v>600,00</v>
       </c>
-      <c r="C144" t="str">
-        <v>-</v>
-      </c>
       <c r="D144" t="str">
+        <v>-</v>
+      </c>
+      <c r="E144" t="str">
         <v>548,54</v>
       </c>
-      <c r="E144" t="str">
-        <v>-</v>
-      </c>
       <c r="F144" t="str">
+        <v>-</v>
+      </c>
+      <c r="G144" t="str">
         <v>589,14</v>
       </c>
-      <c r="G144" t="str">
+      <c r="H144" t="str">
         <v>-</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="str">
+        <v>02-08-2024</v>
+      </c>
+      <c r="B145" t="str">
         <v>Suma</v>
       </c>
-      <c r="B145" t="str">
+      <c r="C145" t="str">
         <v/>
       </c>
-      <c r="C145" t="str">
+      <c r="D145" t="str">
         <v>74 929,3</v>
       </c>
-      <c r="D145" t="str">
+      <c r="E145" t="str">
         <v/>
       </c>
-      <c r="E145" t="str">
+      <c r="F145" t="str">
         <v>34 717,2</v>
       </c>
-      <c r="F145" t="str">
+      <c r="G145" t="str">
         <v/>
       </c>
-      <c r="G145" t="str">
+      <c r="H145" t="str">
         <v>270,3</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G145"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H145"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
almost done, second row cut incorrectly
</commit_message>
<xml_diff>
--- a/tabela.xlsx
+++ b/tabela.xlsx
@@ -406,7 +406,9 @@
     <col min="2" max="2" width="5.83203125" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -420,9 +422,15 @@
         <v>FIXING I</v>
       </c>
       <c r="D1" t="str">
+        <v/>
+      </c>
+      <c r="E1" t="str">
         <v>FIXING II</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
+        <v/>
+      </c>
+      <c r="G1" t="str">
         <v>Notowania ciągłe</v>
       </c>
     </row>

</xml_diff>

<commit_message>
First version without checking dates created
</commit_message>
<xml_diff>
--- a/tabela.xlsx
+++ b/tabela.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -407,6 +407,7 @@
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -422,6 +423,9 @@
       <c r="D1" s="4" t="str">
         <v/>
       </c>
+      <c r="E1" s="4" t="str">
+        <v/>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="str">
@@ -436,22 +440,28 @@
       <c r="D2" s="4" t="str">
         <v/>
       </c>
+      <c r="E2" s="4" t="str">
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="str">
         <v/>
       </c>
       <c r="B3" s="3" t="str">
-        <v>04-07-2024</v>
+        <v>28-08-2024</v>
       </c>
       <c r="C3" s="3" t="str">
-        <v>05-07-2024</v>
+        <v>29-08-2024</v>
       </c>
       <c r="D3" s="3" t="str">
-        <v>06-07-2024</v>
+        <v>30-08-2024</v>
       </c>
       <c r="E3" s="3" t="str">
-        <v>07-07-2024</v>
+        <v>31-08-2024</v>
+      </c>
+      <c r="F3" s="3" t="str">
+        <v>01-09-2024</v>
       </c>
     </row>
     <row r="4">
@@ -459,16 +469,19 @@
         <v>0-1</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>535,00</v>
+        <v>410,00</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>496,00</v>
+        <v>413,70</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>500,00</v>
+        <v>522,00</v>
       </c>
       <c r="E4" s="4" t="str">
-        <v>299,99</v>
+        <v>482,00</v>
+      </c>
+      <c r="F4" s="4" t="str">
+        <v>450,00</v>
       </c>
     </row>
     <row r="5">
@@ -476,16 +489,19 @@
         <v>1-2</v>
       </c>
       <c r="B5" s="4" t="str">
-        <v>438,00</v>
+        <v>388,00</v>
       </c>
       <c r="C5" s="4" t="str">
-        <v>392,00</v>
+        <v>384,73</v>
       </c>
       <c r="D5" s="4" t="str">
-        <v>422,78</v>
+        <v>450,96</v>
       </c>
       <c r="E5" s="4" t="str">
-        <v>303,99</v>
+        <v>450,00</v>
+      </c>
+      <c r="F5" s="4" t="str">
+        <v>420,00</v>
       </c>
     </row>
     <row r="6">
@@ -493,16 +509,19 @@
         <v>2-3</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>407,69</v>
+        <v>376,80</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>390,00</v>
+        <v>367,53</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>390,00</v>
+        <v>427,60</v>
       </c>
       <c r="E6" s="4" t="str">
-        <v>318,00</v>
+        <v>429,60</v>
+      </c>
+      <c r="F6" s="4" t="str">
+        <v>396,00</v>
       </c>
     </row>
     <row r="7">
@@ -510,16 +529,19 @@
         <v>3-4</v>
       </c>
       <c r="B7" s="4" t="str">
-        <v>402,00</v>
+        <v>370,80</v>
       </c>
       <c r="C7" s="4" t="str">
-        <v>394,00</v>
+        <v>376,71</v>
       </c>
       <c r="D7" s="4" t="str">
-        <v>391,10</v>
+        <v>425,00</v>
       </c>
       <c r="E7" s="4" t="str">
-        <v>321,99</v>
+        <v>418,90</v>
+      </c>
+      <c r="F7" s="4" t="str">
+        <v>392,00</v>
       </c>
     </row>
     <row r="8">
@@ -527,16 +549,19 @@
         <v>4-5</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>406,00</v>
+        <v>383,30</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>386,00</v>
+        <v>390,00</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>390,00</v>
+        <v>440,00</v>
       </c>
       <c r="E8" s="4" t="str">
-        <v>323,99</v>
+        <v>413,23</v>
+      </c>
+      <c r="F8" s="4" t="str">
+        <v>398,00</v>
       </c>
     </row>
     <row r="9">
@@ -544,16 +569,19 @@
         <v>5-6</v>
       </c>
       <c r="B9" s="4" t="str">
-        <v>424,69</v>
+        <v>402,00</v>
       </c>
       <c r="C9" s="4" t="str">
-        <v>394,00</v>
+        <v>415,96</v>
       </c>
       <c r="D9" s="4" t="str">
-        <v>406,00</v>
+        <v>490,00</v>
       </c>
       <c r="E9" s="4" t="str">
-        <v>320,00</v>
+        <v>457,80</v>
+      </c>
+      <c r="F9" s="4" t="str">
+        <v>403,70</v>
       </c>
     </row>
     <row r="10">
@@ -561,16 +589,19 @@
         <v>6-7</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>546,00</v>
+        <v>520,00</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>496,00</v>
+        <v>550,00</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>415,69</v>
+        <v>657,31</v>
       </c>
       <c r="E10" s="4" t="str">
-        <v>320,00</v>
+        <v>481,43</v>
+      </c>
+      <c r="F10" s="4" t="str">
+        <v>400,00</v>
       </c>
     </row>
     <row r="11">
@@ -578,16 +609,19 @@
         <v>7-8</v>
       </c>
       <c r="B11" s="4" t="str">
-        <v>455,00</v>
+        <v>530,00</v>
       </c>
       <c r="C11" s="4" t="str">
-        <v>364,06</v>
+        <v>572,36</v>
       </c>
       <c r="D11" s="4" t="str">
-        <v>380,00</v>
+        <v>700,00</v>
       </c>
       <c r="E11" s="4" t="str">
-        <v>305,99</v>
+        <v>492,00</v>
+      </c>
+      <c r="F11" s="4" t="str">
+        <v>397,60</v>
       </c>
     </row>
     <row r="12">
@@ -595,16 +629,19 @@
         <v>8-9</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>390,00</v>
+        <v>479,10</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>320,00</v>
+        <v>478,89</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v>339,40</v>
+        <v>570,00</v>
       </c>
       <c r="E12" s="4" t="str">
-        <v>240,00</v>
+        <v>460,00</v>
+      </c>
+      <c r="F12" s="4" t="str">
+        <v>306,90</v>
       </c>
     </row>
     <row r="13">
@@ -612,16 +649,19 @@
         <v>9-10</v>
       </c>
       <c r="B13" s="4" t="str">
-        <v>352,40</v>
+        <v>382,60</v>
       </c>
       <c r="C13" s="4" t="str">
-        <v>170,00</v>
+        <v>378,50</v>
       </c>
       <c r="D13" s="4" t="str">
-        <v>148,88</v>
+        <v>455,79</v>
       </c>
       <c r="E13" s="4" t="str">
-        <v>150,00</v>
+        <v>353,20</v>
+      </c>
+      <c r="F13" s="4" t="str">
+        <v>80,00</v>
       </c>
     </row>
     <row r="14">
@@ -629,16 +669,19 @@
         <v>10-11</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>275,99</v>
+        <v>259,99</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>1,00</v>
+        <v>230,00</v>
       </c>
       <c r="D14" s="4" t="str">
-        <v>-10,00</v>
+        <v>349,23</v>
       </c>
       <c r="E14" s="4" t="str">
-        <v>150,00</v>
+        <v>190,00</v>
+      </c>
+      <c r="F14" s="4" t="str">
+        <v>0,01</v>
       </c>
     </row>
     <row r="15">
@@ -646,16 +689,19 @@
         <v>11-12</v>
       </c>
       <c r="B15" s="4" t="str">
-        <v>319,99</v>
+        <v>150,00</v>
       </c>
       <c r="C15" s="4" t="str">
-        <v>0,00</v>
+        <v>150,00</v>
       </c>
       <c r="D15" s="4" t="str">
-        <v>-80,00</v>
+        <v>310,11</v>
       </c>
       <c r="E15" s="4" t="str">
-        <v>150,00</v>
+        <v>65,30</v>
+      </c>
+      <c r="F15" s="4" t="str">
+        <v>-53,50</v>
       </c>
     </row>
     <row r="16">
@@ -663,16 +709,19 @@
         <v>12-13</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>305,00</v>
+        <v>70,00</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>0,00</v>
+        <v>85,99</v>
       </c>
       <c r="D16" s="4" t="str">
-        <v>-175,00</v>
+        <v>273,99</v>
       </c>
       <c r="E16" s="4" t="str">
-        <v>120,00</v>
+        <v>9,36</v>
+      </c>
+      <c r="F16" s="4" t="str">
+        <v>-96,56</v>
       </c>
     </row>
     <row r="17">
@@ -680,16 +729,19 @@
         <v>13-14</v>
       </c>
       <c r="B17" s="4" t="str">
-        <v>306,76</v>
+        <v>55,00</v>
       </c>
       <c r="C17" s="4" t="str">
-        <v>0,01</v>
+        <v>50,00</v>
       </c>
       <c r="D17" s="4" t="str">
-        <v>-175,00</v>
+        <v>277,99</v>
       </c>
       <c r="E17" s="4" t="str">
-        <v>175,00</v>
+        <v>0,00</v>
+      </c>
+      <c r="F17" s="4" t="str">
+        <v>-175,49</v>
       </c>
     </row>
     <row r="18">
@@ -697,16 +749,19 @@
         <v>14-15</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>301,99</v>
+        <v>90,00</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>5,00</v>
+        <v>108,88</v>
       </c>
       <c r="D18" s="4" t="str">
-        <v>-175,00</v>
+        <v>319,20</v>
       </c>
       <c r="E18" s="4" t="str">
-        <v>233,40</v>
+        <v>1,00</v>
+      </c>
+      <c r="F18" s="4" t="str">
+        <v>-131,37</v>
       </c>
     </row>
     <row r="19">
@@ -714,16 +769,19 @@
         <v>15-16</v>
       </c>
       <c r="B19" s="4" t="str">
-        <v>267,99</v>
+        <v>282,89</v>
       </c>
       <c r="C19" s="4" t="str">
-        <v>200,00</v>
+        <v>288,00</v>
       </c>
       <c r="D19" s="4" t="str">
-        <v>-120,00</v>
+        <v>398,00</v>
       </c>
       <c r="E19" s="4" t="str">
-        <v>388,00</v>
+        <v>211,99</v>
+      </c>
+      <c r="F19" s="4" t="str">
+        <v>-0,02</v>
       </c>
     </row>
     <row r="20">
@@ -731,16 +789,19 @@
         <v>16-17</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>323,60</v>
+        <v>388,49</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v>329,99</v>
+        <v>400,00</v>
       </c>
       <c r="D20" s="4" t="str">
-        <v>0,00</v>
+        <v>552,99</v>
       </c>
       <c r="E20" s="4" t="str">
-        <v>436,10</v>
+        <v>411,00</v>
+      </c>
+      <c r="F20" s="4" t="str">
+        <v>297,99</v>
       </c>
     </row>
     <row r="21">
@@ -748,16 +809,19 @@
         <v>17-18</v>
       </c>
       <c r="B21" s="4" t="str">
-        <v>361,20</v>
+        <v>508,93</v>
       </c>
       <c r="C21" s="4" t="str">
-        <v>353,42</v>
+        <v>627,30</v>
       </c>
       <c r="D21" s="4" t="str">
-        <v>283,99</v>
+        <v>750,00</v>
       </c>
       <c r="E21" s="4" t="str">
-        <v>480,00</v>
+        <v>516,60</v>
+      </c>
+      <c r="F21" s="4" t="str">
+        <v>465,40</v>
       </c>
     </row>
     <row r="22">
@@ -765,16 +829,19 @@
         <v>18-19</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>550,00</v>
+        <v>769,99</v>
       </c>
       <c r="C22" s="4" t="str">
-        <v>537,70</v>
+        <v>1050,00</v>
       </c>
       <c r="D22" s="4" t="str">
-        <v>430,00</v>
+        <v>1471,00</v>
       </c>
       <c r="E22" s="4" t="str">
-        <v>562,00</v>
+        <v>778,40</v>
+      </c>
+      <c r="F22" s="4" t="str">
+        <v>597,00</v>
       </c>
     </row>
     <row r="23">
@@ -782,16 +849,19 @@
         <v>19-20</v>
       </c>
       <c r="B23" s="4" t="str">
-        <v>652,00</v>
+        <v>1050,00</v>
       </c>
       <c r="C23" s="4" t="str">
-        <v>634,00</v>
+        <v>1600,00</v>
       </c>
       <c r="D23" s="4" t="str">
-        <v>460,00</v>
+        <v>2071,18</v>
       </c>
       <c r="E23" s="4" t="str">
-        <v>670,00</v>
+        <v>995,96</v>
+      </c>
+      <c r="F23" s="4" t="str">
+        <v>700,00</v>
       </c>
     </row>
     <row r="24">
@@ -799,16 +869,19 @@
         <v>20-21</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>729,00</v>
+        <v>1050,00</v>
       </c>
       <c r="C24" s="4" t="str">
-        <v>720,00</v>
+        <v>1511,53</v>
       </c>
       <c r="D24" s="4" t="str">
-        <v>480,00</v>
+        <v>2000,00</v>
       </c>
       <c r="E24" s="4" t="str">
-        <v>775,00</v>
+        <v>867,40</v>
+      </c>
+      <c r="F24" s="4" t="str">
+        <v>700,00</v>
       </c>
     </row>
     <row r="25">
@@ -816,16 +889,19 @@
         <v>21-22</v>
       </c>
       <c r="B25" s="4" t="str">
-        <v>576,96</v>
+        <v>540,00</v>
       </c>
       <c r="C25" s="4" t="str">
-        <v>627,10</v>
+        <v>749,77</v>
       </c>
       <c r="D25" s="4" t="str">
-        <v>502,00</v>
+        <v>824,89</v>
       </c>
       <c r="E25" s="4" t="str">
-        <v>803,00</v>
+        <v>668,50</v>
+      </c>
+      <c r="F25" s="4" t="str">
+        <v>542,00</v>
       </c>
     </row>
     <row r="26">
@@ -833,16 +909,19 @@
         <v>22-23</v>
       </c>
       <c r="B26" s="4" t="str">
-        <v>547,00</v>
+        <v>461,10</v>
       </c>
       <c r="C26" s="4" t="str">
-        <v>537,70</v>
+        <v>590,00</v>
       </c>
       <c r="D26" s="4" t="str">
-        <v>476,00</v>
+        <v>561,70</v>
       </c>
       <c r="E26" s="4" t="str">
-        <v>675,00</v>
+        <v>531,83</v>
+      </c>
+      <c r="F26" s="4" t="str">
+        <v>499,98</v>
       </c>
     </row>
     <row r="27">
@@ -850,16 +929,19 @@
         <v>23-24</v>
       </c>
       <c r="B27" s="4" t="str">
-        <v>438,00</v>
+        <v>400,00</v>
       </c>
       <c r="C27" s="4" t="str">
-        <v>469,00</v>
+        <v>488,60</v>
       </c>
       <c r="D27" s="4" t="str">
-        <v>400,00</v>
+        <v>480,00</v>
       </c>
       <c r="E27" s="4" t="str">
-        <v>552,90</v>
+        <v>466,55</v>
+      </c>
+      <c r="F27" s="4" t="str">
+        <v>444,23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
better package.json and gitignore
</commit_message>
<xml_diff>
--- a/tabela.xlsx
+++ b/tabela.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -409,6 +409,8 @@
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -430,6 +432,12 @@
       <c r="F1" s="4" t="str">
         <v/>
       </c>
+      <c r="G1" s="4" t="str">
+        <v/>
+      </c>
+      <c r="H1" s="4" t="str">
+        <v/>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="str">
@@ -450,28 +458,40 @@
       <c r="F2" s="4" t="str">
         <v/>
       </c>
+      <c r="G2" s="4" t="str">
+        <v/>
+      </c>
+      <c r="H2" s="4" t="str">
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="str">
         <v/>
       </c>
       <c r="B3" s="3" t="str">
-        <v>21-09-2024</v>
+        <v>28-07-2024</v>
       </c>
       <c r="C3" s="3" t="str">
-        <v>22-09-2024</v>
+        <v>29-07-2024</v>
       </c>
       <c r="D3" s="3" t="str">
-        <v>23-09-2024</v>
+        <v>30-07-2024</v>
       </c>
       <c r="E3" s="3" t="str">
-        <v>24-09-2024</v>
+        <v>31-07-2024</v>
       </c>
       <c r="F3" s="3" t="str">
-        <v>25-09-2024</v>
+        <v>01-08-2024</v>
       </c>
       <c r="G3" s="3" t="str">
-        <v>26-09-2024</v>
+        <v>02-08-2024</v>
+      </c>
+      <c r="H3" s="3" t="str">
+        <v>03-08-2024</v>
+      </c>
+      <c r="I3" s="3" t="str">
+        <v>04-08-2024</v>
       </c>
     </row>
     <row r="4">
@@ -479,22 +499,28 @@
         <v>0-1</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>410,00</v>
+        <v>495,36</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>420,00</v>
+        <v>317,99</v>
       </c>
       <c r="D4" s="4" t="str">
-        <v>410,00</v>
+        <v>433,00</v>
       </c>
       <c r="E4" s="4" t="str">
-        <v>395,02</v>
+        <v>473,14</v>
       </c>
       <c r="F4" s="4" t="str">
-        <v>245,86</v>
+        <v>450,00</v>
       </c>
       <c r="G4" s="4" t="str">
-        <v>338,95</v>
+        <v>465,00</v>
+      </c>
+      <c r="H4" s="4" t="str">
+        <v>490,00</v>
+      </c>
+      <c r="I4" s="4" t="str">
+        <v>442,00</v>
       </c>
     </row>
     <row r="5">
@@ -502,22 +528,28 @@
         <v>1-2</v>
       </c>
       <c r="B5" s="4" t="str">
-        <v>388,00</v>
+        <v>439,80</v>
       </c>
       <c r="C5" s="4" t="str">
-        <v>391,00</v>
+        <v>280,00</v>
       </c>
       <c r="D5" s="4" t="str">
-        <v>398,20</v>
+        <v>380,00</v>
       </c>
       <c r="E5" s="4" t="str">
-        <v>371,85</v>
+        <v>418,00</v>
       </c>
       <c r="F5" s="4" t="str">
-        <v>203,34</v>
+        <v>400,00</v>
       </c>
       <c r="G5" s="4" t="str">
-        <v>291,48</v>
+        <v>400,00</v>
+      </c>
+      <c r="H5" s="4" t="str">
+        <v>450,00</v>
+      </c>
+      <c r="I5" s="4" t="str">
+        <v>412,45</v>
       </c>
     </row>
     <row r="6">
@@ -525,22 +557,28 @@
         <v>2-3</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>380,00</v>
+        <v>399,00</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>370,85</v>
+        <v>251,00</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>380,00</v>
+        <v>389,50</v>
       </c>
       <c r="E6" s="4" t="str">
-        <v>365,00</v>
+        <v>406,26</v>
       </c>
       <c r="F6" s="4" t="str">
-        <v>176,52</v>
+        <v>390,00</v>
       </c>
       <c r="G6" s="4" t="str">
-        <v>277,99</v>
+        <v>392,00</v>
+      </c>
+      <c r="H6" s="4" t="str">
+        <v>424,41</v>
+      </c>
+      <c r="I6" s="4" t="str">
+        <v>384,00</v>
       </c>
     </row>
     <row r="7">
@@ -548,22 +586,28 @@
         <v>3-4</v>
       </c>
       <c r="B7" s="4" t="str">
-        <v>388,50</v>
+        <v>400,00</v>
       </c>
       <c r="C7" s="4" t="str">
-        <v>372,00</v>
+        <v>250,00</v>
       </c>
       <c r="D7" s="4" t="str">
-        <v>380,00</v>
+        <v>376,00</v>
       </c>
       <c r="E7" s="4" t="str">
-        <v>370,00</v>
+        <v>407,00</v>
       </c>
       <c r="F7" s="4" t="str">
-        <v>175,07</v>
+        <v>390,00</v>
       </c>
       <c r="G7" s="4" t="str">
-        <v>283,99</v>
+        <v>388,00</v>
+      </c>
+      <c r="H7" s="4" t="str">
+        <v>436,90</v>
+      </c>
+      <c r="I7" s="4" t="str">
+        <v>375,00</v>
       </c>
     </row>
     <row r="8">
@@ -571,22 +615,28 @@
         <v>4-5</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>385,17</v>
+        <v>394,00</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>375,00</v>
+        <v>272,00</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>393,00</v>
+        <v>381,08</v>
       </c>
       <c r="E8" s="4" t="str">
-        <v>372,41</v>
+        <v>408,00</v>
       </c>
       <c r="F8" s="4" t="str">
-        <v>246,59</v>
+        <v>397,20</v>
       </c>
       <c r="G8" s="4" t="str">
-        <v>290,00</v>
+        <v>390,00</v>
+      </c>
+      <c r="H8" s="4" t="str">
+        <v>428,00</v>
+      </c>
+      <c r="I8" s="4" t="str">
+        <v>386,00</v>
       </c>
     </row>
     <row r="9">
@@ -594,22 +644,28 @@
         <v>5-6</v>
       </c>
       <c r="B9" s="4" t="str">
-        <v>399,00</v>
+        <v>382,00</v>
       </c>
       <c r="C9" s="4" t="str">
-        <v>389,00</v>
+        <v>298,00</v>
       </c>
       <c r="D9" s="4" t="str">
-        <v>430,00</v>
+        <v>393,55</v>
       </c>
       <c r="E9" s="4" t="str">
-        <v>410,00</v>
+        <v>443,55</v>
       </c>
       <c r="F9" s="4" t="str">
-        <v>324,70</v>
+        <v>437,00</v>
       </c>
       <c r="G9" s="4" t="str">
-        <v>360,00</v>
+        <v>431,28</v>
+      </c>
+      <c r="H9" s="4" t="str">
+        <v>447,91</v>
+      </c>
+      <c r="I9" s="4" t="str">
+        <v>392,00</v>
       </c>
     </row>
     <row r="10">
@@ -617,22 +673,28 @@
         <v>6-7</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>450,19</v>
+        <v>412,00</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>390,27</v>
+        <v>406,00</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>680,00</v>
+        <v>509,11</v>
       </c>
       <c r="E10" s="4" t="str">
         <v>550,00</v>
       </c>
       <c r="F10" s="4" t="str">
-        <v>448,00</v>
+        <v>530,00</v>
       </c>
       <c r="G10" s="4" t="str">
-        <v>433,00</v>
+        <v>542,00</v>
+      </c>
+      <c r="H10" s="4" t="str">
+        <v>480,00</v>
+      </c>
+      <c r="I10" s="4" t="str">
+        <v>396,00</v>
       </c>
     </row>
     <row r="11">
@@ -640,22 +702,28 @@
         <v>7-8</v>
       </c>
       <c r="B11" s="4" t="str">
-        <v>490,00</v>
+        <v>390,00</v>
       </c>
       <c r="C11" s="4" t="str">
-        <v>400,00</v>
+        <v>378,00</v>
       </c>
       <c r="D11" s="4" t="str">
-        <v>769,00</v>
+        <v>506,40</v>
       </c>
       <c r="E11" s="4" t="str">
-        <v>680,00</v>
+        <v>530,00</v>
       </c>
       <c r="F11" s="4" t="str">
-        <v>458,90</v>
+        <v>520,00</v>
       </c>
       <c r="G11" s="4" t="str">
-        <v>435,20</v>
+        <v>540,00</v>
+      </c>
+      <c r="H11" s="4" t="str">
+        <v>488,68</v>
+      </c>
+      <c r="I11" s="4" t="str">
+        <v>359,00</v>
       </c>
     </row>
     <row r="12">
@@ -663,22 +731,28 @@
         <v>8-9</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>480,00</v>
+        <v>361,04</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>329,99</v>
+        <v>299,00</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v>600,00</v>
+        <v>416,30</v>
       </c>
       <c r="E12" s="4" t="str">
-        <v>538,00</v>
+        <v>420,00</v>
       </c>
       <c r="F12" s="4" t="str">
-        <v>419,60</v>
+        <v>432,41</v>
       </c>
       <c r="G12" s="4" t="str">
-        <v>377,66</v>
+        <v>488,50</v>
+      </c>
+      <c r="H12" s="4" t="str">
+        <v>524,27</v>
+      </c>
+      <c r="I12" s="4" t="str">
+        <v>259,99</v>
       </c>
     </row>
     <row r="13">
@@ -686,22 +760,28 @@
         <v>9-10</v>
       </c>
       <c r="B13" s="4" t="str">
-        <v>303,80</v>
+        <v>269,99</v>
       </c>
       <c r="C13" s="4" t="str">
-        <v>218,24</v>
+        <v>137,99</v>
       </c>
       <c r="D13" s="4" t="str">
-        <v>467,00</v>
+        <v>283,99</v>
       </c>
       <c r="E13" s="4" t="str">
-        <v>436,60</v>
+        <v>303,99</v>
       </c>
       <c r="F13" s="4" t="str">
-        <v>327,99</v>
+        <v>355,57</v>
       </c>
       <c r="G13" s="4" t="str">
-        <v>315,99</v>
+        <v>450,00</v>
+      </c>
+      <c r="H13" s="4" t="str">
+        <v>406,00</v>
+      </c>
+      <c r="I13" s="4" t="str">
+        <v>101,00</v>
       </c>
     </row>
     <row r="14">
@@ -709,22 +789,28 @@
         <v>10-11</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>133,00</v>
+        <v>100,00</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>40,00</v>
+        <v>0,00</v>
       </c>
       <c r="D14" s="4" t="str">
-        <v>384,00</v>
+        <v>180,11</v>
       </c>
       <c r="E14" s="4" t="str">
-        <v>354,83</v>
+        <v>198,12</v>
       </c>
       <c r="F14" s="4" t="str">
-        <v>199,99</v>
+        <v>288,00</v>
       </c>
       <c r="G14" s="4" t="str">
-        <v>262,70</v>
+        <v>404,00</v>
+      </c>
+      <c r="H14" s="4" t="str">
+        <v>388,80</v>
+      </c>
+      <c r="I14" s="4" t="str">
+        <v>30,00</v>
       </c>
     </row>
     <row r="15">
@@ -732,22 +818,28 @@
         <v>11-12</v>
       </c>
       <c r="B15" s="4" t="str">
-        <v>1,00</v>
+        <v>0,00</v>
       </c>
       <c r="C15" s="4" t="str">
-        <v>-9,59</v>
+        <v>-31,00</v>
       </c>
       <c r="D15" s="4" t="str">
-        <v>350,00</v>
+        <v>90,11</v>
       </c>
       <c r="E15" s="4" t="str">
-        <v>276,40</v>
+        <v>105,95</v>
       </c>
       <c r="F15" s="4" t="str">
-        <v>108,74</v>
+        <v>263,40</v>
       </c>
       <c r="G15" s="4" t="str">
-        <v>164,04</v>
+        <v>390,34</v>
+      </c>
+      <c r="H15" s="4" t="str">
+        <v>377,76</v>
+      </c>
+      <c r="I15" s="4" t="str">
+        <v>45,99</v>
       </c>
     </row>
     <row r="16">
@@ -755,22 +847,28 @@
         <v>12-13</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>-3,36</v>
+        <v>-30,01</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>-66,83</v>
+        <v>-55,00</v>
       </c>
       <c r="D16" s="4" t="str">
-        <v>316,20</v>
+        <v>30,00</v>
       </c>
       <c r="E16" s="4" t="str">
-        <v>242,22</v>
+        <v>70,00</v>
       </c>
       <c r="F16" s="4" t="str">
-        <v>90,00</v>
+        <v>235,90</v>
       </c>
       <c r="G16" s="4" t="str">
-        <v>106,30</v>
+        <v>387,59</v>
+      </c>
+      <c r="H16" s="4" t="str">
+        <v>361,40</v>
+      </c>
+      <c r="I16" s="4" t="str">
+        <v>79,99</v>
       </c>
     </row>
     <row r="17">
@@ -778,22 +876,28 @@
         <v>13-14</v>
       </c>
       <c r="B17" s="4" t="str">
-        <v>-1,42</v>
+        <v>-71,01</v>
       </c>
       <c r="C17" s="4" t="str">
-        <v>-62,01</v>
+        <v>-54,01</v>
       </c>
       <c r="D17" s="4" t="str">
-        <v>309,80</v>
+        <v>10,11</v>
       </c>
       <c r="E17" s="4" t="str">
-        <v>227,99</v>
+        <v>70,00</v>
       </c>
       <c r="F17" s="4" t="str">
-        <v>109,99</v>
+        <v>241,99</v>
       </c>
       <c r="G17" s="4" t="str">
-        <v>82,19</v>
+        <v>394,00</v>
+      </c>
+      <c r="H17" s="4" t="str">
+        <v>326,70</v>
+      </c>
+      <c r="I17" s="4" t="str">
+        <v>199,89</v>
       </c>
     </row>
     <row r="18">
@@ -801,22 +905,28 @@
         <v>14-15</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>1,00</v>
+        <v>-190,00</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>-3,35</v>
+        <v>-30,01</v>
       </c>
       <c r="D18" s="4" t="str">
-        <v>336,51</v>
+        <v>21,40</v>
       </c>
       <c r="E18" s="4" t="str">
-        <v>250,00</v>
+        <v>100,00</v>
       </c>
       <c r="F18" s="4" t="str">
-        <v>184,00</v>
+        <v>233,99</v>
       </c>
       <c r="G18" s="4" t="str">
-        <v>119,00</v>
+        <v>406,00</v>
+      </c>
+      <c r="H18" s="4" t="str">
+        <v>300,00</v>
+      </c>
+      <c r="I18" s="4" t="str">
+        <v>217,99</v>
       </c>
     </row>
     <row r="19">
@@ -824,22 +934,28 @@
         <v>15-16</v>
       </c>
       <c r="B19" s="4" t="str">
-        <v>175,00</v>
+        <v>-176,00</v>
       </c>
       <c r="C19" s="4" t="str">
-        <v>60,00</v>
+        <v>0,01</v>
       </c>
       <c r="D19" s="4" t="str">
-        <v>383,00</v>
+        <v>165,00</v>
       </c>
       <c r="E19" s="4" t="str">
-        <v>300,00</v>
+        <v>239,99</v>
       </c>
       <c r="F19" s="4" t="str">
-        <v>300,01</v>
+        <v>295,67</v>
       </c>
       <c r="G19" s="4" t="str">
-        <v>201,48</v>
+        <v>482,86</v>
+      </c>
+      <c r="H19" s="4" t="str">
+        <v>340,00</v>
+      </c>
+      <c r="I19" s="4" t="str">
+        <v>330,27</v>
       </c>
     </row>
     <row r="20">
@@ -847,22 +963,28 @@
         <v>16-17</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>480,00</v>
+        <v>-111,00</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v>368,72</v>
+        <v>90,00</v>
       </c>
       <c r="D20" s="4" t="str">
-        <v>475,00</v>
+        <v>315,99</v>
       </c>
       <c r="E20" s="4" t="str">
+        <v>370,60</v>
+      </c>
+      <c r="F20" s="4" t="str">
+        <v>385,69</v>
+      </c>
+      <c r="G20" s="4" t="str">
+        <v>482,86</v>
+      </c>
+      <c r="H20" s="4" t="str">
         <v>399,99</v>
       </c>
-      <c r="F20" s="4" t="str">
-        <v>416,00</v>
-      </c>
-      <c r="G20" s="4" t="str">
-        <v>280,00</v>
+      <c r="I20" s="4" t="str">
+        <v>386,00</v>
       </c>
     </row>
     <row r="21">
@@ -870,22 +992,28 @@
         <v>17-18</v>
       </c>
       <c r="B21" s="4" t="str">
-        <v>576,00</v>
+        <v>-15,00</v>
       </c>
       <c r="C21" s="4" t="str">
-        <v>510,00</v>
+        <v>281,99</v>
       </c>
       <c r="D21" s="4" t="str">
-        <v>688,87</v>
+        <v>380,60</v>
       </c>
       <c r="E21" s="4" t="str">
-        <v>475,00</v>
+        <v>379,00</v>
       </c>
       <c r="F21" s="4" t="str">
-        <v>489,70</v>
+        <v>444,97</v>
       </c>
       <c r="G21" s="4" t="str">
-        <v>320,00</v>
+        <v>469,00</v>
+      </c>
+      <c r="H21" s="4" t="str">
+        <v>492,90</v>
+      </c>
+      <c r="I21" s="4" t="str">
+        <v>482,00</v>
       </c>
     </row>
     <row r="22">
@@ -893,22 +1021,28 @@
         <v>18-19</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>794,00</v>
+        <v>159,30</v>
       </c>
       <c r="C22" s="4" t="str">
-        <v>740,00</v>
+        <v>380,00</v>
       </c>
       <c r="D22" s="4" t="str">
-        <v>949,00</v>
+        <v>481,00</v>
       </c>
       <c r="E22" s="4" t="str">
-        <v>549,31</v>
+        <v>499,40</v>
       </c>
       <c r="F22" s="4" t="str">
-        <v>669,95</v>
+        <v>503,60</v>
       </c>
       <c r="G22" s="4" t="str">
-        <v>380,00</v>
+        <v>549,00</v>
+      </c>
+      <c r="H22" s="4" t="str">
+        <v>490,00</v>
+      </c>
+      <c r="I22" s="4" t="str">
+        <v>465,00</v>
       </c>
     </row>
     <row r="23">
@@ -916,22 +1050,28 @@
         <v>19-20</v>
       </c>
       <c r="B23" s="4" t="str">
-        <v>900,00</v>
+        <v>343,40</v>
       </c>
       <c r="C23" s="4" t="str">
-        <v>900,00</v>
+        <v>558,00</v>
       </c>
       <c r="D23" s="4" t="str">
-        <v>1299,00</v>
+        <v>682,00</v>
       </c>
       <c r="E23" s="4" t="str">
-        <v>639,00</v>
+        <v>632,00</v>
       </c>
       <c r="F23" s="4" t="str">
-        <v>850,00</v>
+        <v>612,00</v>
       </c>
       <c r="G23" s="4" t="str">
-        <v>428,44</v>
+        <v>600,00</v>
+      </c>
+      <c r="H23" s="4" t="str">
+        <v>560,00</v>
+      </c>
+      <c r="I23" s="4" t="str">
+        <v>489,00</v>
       </c>
     </row>
     <row r="24">
@@ -939,22 +1079,28 @@
         <v>20-21</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>640,00</v>
+        <v>420,80</v>
       </c>
       <c r="C24" s="4" t="str">
-        <v>675,00</v>
+        <v>680,00</v>
       </c>
       <c r="D24" s="4" t="str">
-        <v>695,70</v>
+        <v>853,40</v>
       </c>
       <c r="E24" s="4" t="str">
-        <v>490,30</v>
+        <v>825,00</v>
       </c>
       <c r="F24" s="4" t="str">
+        <v>738,99</v>
+      </c>
+      <c r="G24" s="4" t="str">
+        <v>670,00</v>
+      </c>
+      <c r="H24" s="4" t="str">
         <v>600,00</v>
       </c>
-      <c r="G24" s="4" t="str">
-        <v>389,00</v>
+      <c r="I24" s="4" t="str">
+        <v>537,44</v>
       </c>
     </row>
     <row r="25">
@@ -962,22 +1108,28 @@
         <v>21-22</v>
       </c>
       <c r="B25" s="4" t="str">
-        <v>492,00</v>
+        <v>445,80</v>
       </c>
       <c r="C25" s="4" t="str">
-        <v>530,00</v>
+        <v>625,00</v>
       </c>
       <c r="D25" s="4" t="str">
-        <v>481,42</v>
+        <v>720,00</v>
       </c>
       <c r="E25" s="4" t="str">
-        <v>395,00</v>
+        <v>634,00</v>
       </c>
       <c r="F25" s="4" t="str">
-        <v>450,00</v>
+        <v>585,00</v>
       </c>
       <c r="G25" s="4" t="str">
-        <v>310,00</v>
+        <v>553,90</v>
+      </c>
+      <c r="H25" s="4" t="str">
+        <v>586,61</v>
+      </c>
+      <c r="I25" s="4" t="str">
+        <v>512,20</v>
       </c>
     </row>
     <row r="26">
@@ -985,22 +1137,28 @@
         <v>22-23</v>
       </c>
       <c r="B26" s="4" t="str">
-        <v>439,00</v>
+        <v>390,00</v>
       </c>
       <c r="C26" s="4" t="str">
-        <v>464,20</v>
+        <v>496,00</v>
       </c>
       <c r="D26" s="4" t="str">
-        <v>424,00</v>
+        <v>549,00</v>
       </c>
       <c r="E26" s="4" t="str">
-        <v>379,00</v>
+        <v>520,00</v>
       </c>
       <c r="F26" s="4" t="str">
-        <v>407,00</v>
+        <v>537,00</v>
       </c>
       <c r="G26" s="4" t="str">
-        <v>287,99</v>
+        <v>513,70</v>
+      </c>
+      <c r="H26" s="4" t="str">
+        <v>514,80</v>
+      </c>
+      <c r="I26" s="4" t="str">
+        <v>473,61</v>
       </c>
     </row>
     <row r="27">
@@ -1008,22 +1166,28 @@
         <v>23-24</v>
       </c>
       <c r="B27" s="4" t="str">
-        <v>405,90</v>
+        <v>338,80</v>
       </c>
       <c r="C27" s="4" t="str">
-        <v>420,00</v>
+        <v>428,90</v>
       </c>
       <c r="D27" s="4" t="str">
-        <v>375,54</v>
+        <v>458,00</v>
       </c>
       <c r="E27" s="4" t="str">
-        <v>317,99</v>
+        <v>443,80</v>
       </c>
       <c r="F27" s="4" t="str">
-        <v>372,00</v>
+        <v>450,00</v>
       </c>
       <c r="G27" s="4" t="str">
-        <v>201,11</v>
+        <v>449,00</v>
+      </c>
+      <c r="H27" s="4" t="str">
+        <v>441,87</v>
+      </c>
+      <c r="I27" s="4" t="str">
+        <v>437,39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>